<commit_message>
Updated to latest version from Alon Scope.
</commit_message>
<xml_diff>
--- a/basis/Diagnosis_mapper_source.xlsx
+++ b/basis/Diagnosis_mapper_source.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\weberj3\Documents\git\dermodelphi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\weberj3\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAC964CA-8447-4E7F-9E9F-937975E85709}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03CAEA0F-7C6F-49C7-A854-DFBCBBDF758B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -276,6 +276,12 @@
     <t>Basal cell carcinoma with sarcomatoid differentiation</t>
   </si>
   <si>
+    <t xml:space="preserve">Nevus, Unna </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nevus, Miescher </t>
+  </si>
+  <si>
     <t>Blue nevus, NOS</t>
   </si>
   <si>
@@ -579,6 +585,18 @@
     <t>Hemorrhage, Subungual</t>
   </si>
   <si>
+    <t xml:space="preserve">Nevus, Atypical, NOS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nevus, Clark </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nevus, Dysplastic </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nevus, Congenital (per history - present at birth or within 1 year of infancy) </t>
+  </si>
+  <si>
     <t xml:space="preserve">Nevus, Recurrent / persistent </t>
   </si>
   <si>
@@ -738,6 +756,9 @@
     <t>Synonyms</t>
   </si>
   <si>
+    <t xml:space="preserve">Nevus, Spitz </t>
+  </si>
+  <si>
     <t>Nevus, Reed</t>
   </si>
   <si>
@@ -1005,9 +1026,6 @@
     <t>Urticaria pigmentosa</t>
   </si>
   <si>
-    <t>Mastocytosis, Diffuse / multifocal  (subtype: Telangiectasia mcularis eruptiva perstans, Diffuse cutaenous, other; to be specified)</t>
-  </si>
-  <si>
     <t>Mast cell proliferation, other (to be specified)</t>
   </si>
   <si>
@@ -1113,15 +1131,9 @@
     <t>Exogenous, other (to be specified)</t>
   </si>
   <si>
-    <t>Collision / two benign proliferations</t>
-  </si>
-  <si>
     <t>Benign, other (to be specified)</t>
   </si>
   <si>
-    <t>Collision</t>
-  </si>
-  <si>
     <t>Benign - Other or not readily classifiable</t>
   </si>
   <si>
@@ -1365,9 +1377,6 @@
     <t>Skin metastasis of internal solid (non-hematological) cancer</t>
   </si>
   <si>
-    <t>Collision - at least one malignant proliferation</t>
-  </si>
-  <si>
     <t>Primary cutaneous CD30+ lymphoproliferative disease, Cutanous anaplatic large cell lymphoma</t>
   </si>
   <si>
@@ -1407,9 +1416,6 @@
     <t>Malignant, other (or not readily classifiable; to be specified)</t>
   </si>
   <si>
-    <t xml:space="preserve">Nevus, Congenital pattern (per histopathology)  </t>
-  </si>
-  <si>
     <t>Benign adnexal epithelial proliferations, Sebaceous, other (to be specified)</t>
   </si>
   <si>
@@ -1422,6 +1428,9 @@
     <t>Benign soft tissue proliferations, Adipocytic, other (to be specified)</t>
   </si>
   <si>
+    <t xml:space="preserve">Nevus, BAP-1 deficient </t>
+  </si>
+  <si>
     <t>Wiesner nevus</t>
   </si>
   <si>
@@ -1440,31 +1449,22 @@
     <t>Superficial (Ackerman nevus);Superficial and deep (Zitelli nevus);Deep (Mark nevus)</t>
   </si>
   <si>
-    <t>Nevus, Atypical, NOS</t>
-  </si>
-  <si>
-    <t>Nevus, Clark</t>
-  </si>
-  <si>
-    <t>Nevus, Dysplastic</t>
-  </si>
-  <si>
-    <t>Nevus, Spitz</t>
-  </si>
-  <si>
-    <t>Nevus, Unna</t>
-  </si>
-  <si>
-    <t>Nevus, Miescher</t>
-  </si>
-  <si>
-    <t>Nevus, BAP-1 deficient</t>
-  </si>
-  <si>
-    <t>Nevus, Congenital (per history - present at birth or within 1 year of infancy)</t>
-  </si>
-  <si>
-    <t>Malignant - Other (or not readily classifiable)</t>
+    <t>Malignant – Other (or not readily classifiable)</t>
+  </si>
+  <si>
+    <t>Collisions</t>
+  </si>
+  <si>
+    <t>Collisions - at least one malignant proliferation</t>
+  </si>
+  <si>
+    <t>Nevus, Congenital pattern (per histopathology)</t>
+  </si>
+  <si>
+    <t>Mastocytosis, Diffuse / multifocal (subtype: Telangiectasia mcularis eruptiva perstans, Diffuse cutaenous, other; to be specified)</t>
+  </si>
+  <si>
+    <t>Collisions, Two benign proliferations (to be specified)</t>
   </si>
 </sst>
 </file>
@@ -2067,12 +2067,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="18.75"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="50.7109375" customWidth="1"/>
-    <col min="3" max="3" width="80.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="60.7109375" customWidth="1"/>
+    <col min="3" max="3" width="112.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="42.42578125" style="25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="45.5703125" style="25" customWidth="1"/>
-    <col min="6" max="6" width="45.5703125" style="28" customWidth="1"/>
+    <col min="5" max="5" width="84" style="25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="75.5703125" style="28" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="7.5703125" style="40" customWidth="1"/>
     <col min="9" max="9" width="5.7109375" style="41" customWidth="1"/>
     <col min="10" max="10" width="8.7109375" style="40" customWidth="1"/>
@@ -2081,37 +2081,37 @@
   <sheetData>
     <row r="1" spans="1:11" s="37" customFormat="1" ht="19.5" thickBot="1">
       <c r="A1" s="34" t="s">
+        <v>219</v>
+      </c>
+      <c r="B1" s="34" t="s">
         <v>213</v>
       </c>
-      <c r="B1" s="34" t="s">
-        <v>207</v>
-      </c>
       <c r="C1" s="35" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="D1" s="36" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="E1" s="36" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="F1" s="36" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="G1" s="36" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="H1" s="36" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="I1" s="38" t="s">
-        <v>228</v>
+        <v>235</v>
       </c>
       <c r="J1" s="36" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="K1" s="36" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="18.75" customHeight="1">
@@ -2119,10 +2119,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>226</v>
+        <v>233</v>
       </c>
       <c r="D2" s="29"/>
       <c r="E2" s="28"/>
@@ -2149,7 +2149,7 @@
       <c r="A3" s="31"/>
       <c r="B3" s="9"/>
       <c r="C3" s="3" t="s">
-        <v>227</v>
+        <v>234</v>
       </c>
       <c r="D3" s="29"/>
       <c r="E3" s="28"/>
@@ -2174,7 +2174,7 @@
       <c r="A4" s="31"/>
       <c r="B4" s="9"/>
       <c r="C4" s="4" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D4" s="29"/>
       <c r="E4" s="28"/>
@@ -2199,11 +2199,11 @@
       <c r="A5" s="31"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
-        <v>449</v>
+        <v>164</v>
       </c>
       <c r="D5" s="29"/>
       <c r="E5" s="29" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="F5" s="29"/>
       <c r="G5" s="40">
@@ -2230,11 +2230,11 @@
       <c r="A6" s="31"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3" t="s">
-        <v>450</v>
+        <v>165</v>
       </c>
       <c r="D6" s="29"/>
       <c r="E6" s="29" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="F6" s="29"/>
       <c r="G6" s="40">
@@ -2258,11 +2258,11 @@
       <c r="A7" s="31"/>
       <c r="B7" s="3"/>
       <c r="C7" s="4" t="s">
-        <v>451</v>
+        <v>166</v>
       </c>
       <c r="D7" s="29"/>
       <c r="E7" s="29" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="F7" s="29"/>
       <c r="G7" s="40">
@@ -2286,13 +2286,13 @@
       <c r="A8" s="31"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3" t="s">
-        <v>452</v>
+        <v>221</v>
       </c>
       <c r="D8" s="29" t="s">
-        <v>260</v>
+        <v>267</v>
       </c>
       <c r="E8" s="29" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="F8" s="29"/>
       <c r="G8" s="40">
@@ -2319,13 +2319,13 @@
       <c r="A9" s="31"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3" t="s">
-        <v>215</v>
+        <v>222</v>
       </c>
       <c r="D9" s="29" t="s">
-        <v>259</v>
+        <v>266</v>
       </c>
       <c r="E9" s="29" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="F9" s="29"/>
       <c r="G9" s="40">
@@ -2349,11 +2349,11 @@
       <c r="A10" s="31"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3" t="s">
-        <v>453</v>
+        <v>61</v>
       </c>
       <c r="D10" s="29"/>
       <c r="E10" s="29" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="F10" s="29"/>
       <c r="G10" s="40">
@@ -2377,11 +2377,11 @@
       <c r="A11" s="31"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3" t="s">
-        <v>454</v>
+        <v>62</v>
       </c>
       <c r="D11" s="29"/>
       <c r="E11" s="29" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="F11" s="29"/>
       <c r="G11" s="40">
@@ -2405,13 +2405,13 @@
       <c r="A12" s="31"/>
       <c r="B12" s="3"/>
       <c r="C12" s="4" t="s">
-        <v>455</v>
+        <v>445</v>
       </c>
       <c r="D12" s="29" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="E12" s="29" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="F12" s="29"/>
       <c r="G12" s="40">
@@ -2435,14 +2435,14 @@
       <c r="A13" s="31"/>
       <c r="B13" s="3"/>
       <c r="C13" s="5" t="s">
-        <v>456</v>
+        <v>167</v>
       </c>
       <c r="D13" s="29"/>
       <c r="E13" s="29" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="F13" s="29" t="s">
-        <v>448</v>
+        <v>451</v>
       </c>
       <c r="G13" s="40">
         <f t="shared" si="0"/>
@@ -2468,14 +2468,14 @@
       <c r="A14" s="31"/>
       <c r="B14" s="3"/>
       <c r="C14" s="6" t="s">
-        <v>438</v>
+        <v>455</v>
       </c>
       <c r="D14" s="29"/>
       <c r="E14" s="29" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="F14" s="29" t="s">
-        <v>448</v>
+        <v>451</v>
       </c>
       <c r="G14" s="40">
         <f t="shared" si="0"/>
@@ -2498,7 +2498,7 @@
       <c r="A15" s="31"/>
       <c r="B15" s="3"/>
       <c r="C15" s="5" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D15" s="29"/>
       <c r="E15" s="28"/>
@@ -2526,7 +2526,7 @@
       <c r="A16" s="31"/>
       <c r="B16" s="3"/>
       <c r="C16" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D16" s="29"/>
       <c r="E16" s="28"/>
@@ -2551,7 +2551,7 @@
       <c r="A17" s="31"/>
       <c r="B17" s="3"/>
       <c r="C17" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D17" s="29"/>
       <c r="E17" s="28"/>
@@ -2579,10 +2579,10 @@
       <c r="A18" s="31"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3" t="s">
-        <v>217</v>
+        <v>224</v>
       </c>
       <c r="D18" s="29" t="s">
-        <v>216</v>
+        <v>223</v>
       </c>
       <c r="E18" s="28"/>
       <c r="G18" s="40">
@@ -2606,10 +2606,10 @@
       <c r="A19" s="31"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3" t="s">
-        <v>218</v>
+        <v>225</v>
       </c>
       <c r="D19" s="29" t="s">
-        <v>219</v>
+        <v>226</v>
       </c>
       <c r="E19" s="28"/>
       <c r="G19" s="40">
@@ -2633,7 +2633,7 @@
       <c r="A20" s="31"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D20" s="29"/>
       <c r="E20" s="28"/>
@@ -2658,10 +2658,10 @@
       <c r="A21" s="31"/>
       <c r="B21" s="3"/>
       <c r="C21" s="4" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
       <c r="D21" s="29" t="s">
-        <v>221</v>
+        <v>228</v>
       </c>
       <c r="E21" s="28"/>
       <c r="G21" s="40">
@@ -2685,7 +2685,7 @@
       <c r="A22" s="31"/>
       <c r="B22" s="3"/>
       <c r="C22" s="5" t="s">
-        <v>222</v>
+        <v>229</v>
       </c>
       <c r="D22" s="29"/>
       <c r="E22" s="28"/>
@@ -2713,7 +2713,7 @@
       <c r="A23" s="31"/>
       <c r="B23" s="3"/>
       <c r="C23" s="6" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D23" s="29"/>
       <c r="E23" s="28"/>
@@ -2738,11 +2738,11 @@
       <c r="A24" s="31"/>
       <c r="B24" s="3"/>
       <c r="C24" s="5" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="D24" s="29"/>
       <c r="E24" s="29" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="F24" s="29"/>
       <c r="G24" s="40">
@@ -2769,11 +2769,11 @@
       <c r="A25" s="31"/>
       <c r="B25" s="3"/>
       <c r="C25" s="7" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="D25" s="29"/>
       <c r="E25" s="29" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="F25" s="29"/>
       <c r="G25" s="40">
@@ -2797,11 +2797,11 @@
       <c r="A26" s="31"/>
       <c r="B26" s="3"/>
       <c r="C26" s="7" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="D26" s="29"/>
       <c r="E26" s="29" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="F26" s="29"/>
       <c r="G26" s="40">
@@ -2825,13 +2825,13 @@
       <c r="A27" s="31"/>
       <c r="B27" s="3"/>
       <c r="C27" s="7" t="s">
-        <v>229</v>
+        <v>236</v>
       </c>
       <c r="D27" s="29" t="s">
-        <v>230</v>
+        <v>237</v>
       </c>
       <c r="E27" s="29" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="F27" s="29"/>
       <c r="G27" s="40">
@@ -2855,11 +2855,11 @@
       <c r="A28" s="31"/>
       <c r="B28" s="3"/>
       <c r="C28" s="7" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="D28" s="29"/>
       <c r="E28" s="29" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="F28" s="29"/>
       <c r="G28" s="40">
@@ -2883,13 +2883,13 @@
       <c r="A29" s="31"/>
       <c r="B29" s="3"/>
       <c r="C29" s="7" t="s">
-        <v>223</v>
+        <v>230</v>
       </c>
       <c r="D29" s="29" t="s">
-        <v>224</v>
+        <v>231</v>
       </c>
       <c r="E29" s="29" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="F29" s="29"/>
       <c r="G29" s="40">
@@ -2913,10 +2913,10 @@
       <c r="A30" s="31"/>
       <c r="B30" s="3"/>
       <c r="C30" s="5" t="s">
-        <v>225</v>
+        <v>232</v>
       </c>
       <c r="D30" s="29" t="s">
-        <v>242</v>
+        <v>249</v>
       </c>
       <c r="E30" s="28"/>
       <c r="G30" s="40">
@@ -2971,7 +2971,7 @@
       <c r="A32" s="31"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D32" s="29"/>
       <c r="E32" s="28"/>
@@ -2996,7 +2996,7 @@
       <c r="A33" s="31"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D33" s="29"/>
       <c r="E33" s="28"/>
@@ -3049,7 +3049,7 @@
       <c r="A35" s="31"/>
       <c r="B35" s="3"/>
       <c r="C35" s="2" t="s">
-        <v>247</v>
+        <v>254</v>
       </c>
       <c r="D35" s="29"/>
       <c r="E35" s="28"/>
@@ -3079,10 +3079,10 @@
         <v>1</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>231</v>
+        <v>238</v>
       </c>
       <c r="D36" s="29" t="s">
-        <v>243</v>
+        <v>250</v>
       </c>
       <c r="E36" s="28"/>
       <c r="G36" s="40">
@@ -3109,10 +3109,10 @@
       <c r="A37" s="31"/>
       <c r="B37" s="7"/>
       <c r="C37" s="7" t="s">
-        <v>232</v>
+        <v>239</v>
       </c>
       <c r="D37" s="29" t="s">
-        <v>244</v>
+        <v>251</v>
       </c>
       <c r="E37" s="28"/>
       <c r="G37" s="40">
@@ -3160,10 +3160,10 @@
     <row r="39" spans="1:11" ht="18.75" customHeight="1">
       <c r="A39" s="31"/>
       <c r="B39" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>245</v>
+        <v>252</v>
       </c>
       <c r="D39" s="29"/>
       <c r="E39" s="28"/>
@@ -3216,10 +3216,10 @@
       <c r="A41" s="31"/>
       <c r="B41" s="3"/>
       <c r="C41" s="4" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="D41" s="29" t="s">
-        <v>246</v>
+        <v>253</v>
       </c>
       <c r="E41" s="28"/>
       <c r="G41" s="40">
@@ -3243,10 +3243,10 @@
       <c r="A42" s="31"/>
       <c r="B42" s="3"/>
       <c r="C42" s="2" t="s">
-        <v>234</v>
+        <v>241</v>
       </c>
       <c r="D42" s="29" t="s">
-        <v>235</v>
+        <v>242</v>
       </c>
       <c r="E42" s="28"/>
       <c r="G42" s="40">
@@ -3323,7 +3323,7 @@
       <c r="A45" s="31"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D45" s="29"/>
       <c r="E45" s="28"/>
@@ -3348,7 +3348,7 @@
       <c r="A46" s="31"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D46" s="29"/>
       <c r="E46" s="28"/>
@@ -3373,7 +3373,7 @@
       <c r="A47" s="31"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D47" s="29"/>
       <c r="E47" s="28"/>
@@ -3398,7 +3398,7 @@
       <c r="A48" s="31"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D48" s="29"/>
       <c r="E48" s="28"/>
@@ -3423,7 +3423,7 @@
       <c r="A49" s="31"/>
       <c r="B49" s="4"/>
       <c r="C49" s="4" t="s">
-        <v>248</v>
+        <v>255</v>
       </c>
       <c r="D49" s="29"/>
       <c r="E49" s="28"/>
@@ -3447,10 +3447,10 @@
     <row r="50" spans="1:11" ht="18.75" customHeight="1">
       <c r="A50" s="31"/>
       <c r="B50" s="5" t="s">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D50" s="29"/>
       <c r="E50" s="28"/>
@@ -3478,10 +3478,10 @@
       <c r="A51" s="31"/>
       <c r="B51" s="7"/>
       <c r="C51" s="7" t="s">
-        <v>237</v>
+        <v>244</v>
       </c>
       <c r="D51" s="29" t="s">
-        <v>258</v>
+        <v>265</v>
       </c>
       <c r="E51" s="28"/>
       <c r="G51" s="40">
@@ -3505,7 +3505,7 @@
       <c r="A52" s="31"/>
       <c r="B52" s="7"/>
       <c r="C52" s="7" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D52" s="29"/>
       <c r="E52" s="28"/>
@@ -3530,7 +3530,7 @@
       <c r="A53" s="31"/>
       <c r="B53" s="7"/>
       <c r="C53" s="7" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D53" s="29"/>
       <c r="E53" s="28"/>
@@ -3555,7 +3555,7 @@
       <c r="A54" s="31"/>
       <c r="B54" s="7"/>
       <c r="C54" s="7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D54" s="29"/>
       <c r="E54" s="28"/>
@@ -3580,7 +3580,7 @@
       <c r="A55" s="31"/>
       <c r="B55" s="7"/>
       <c r="C55" s="7" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D55" s="29"/>
       <c r="E55" s="28"/>
@@ -3605,7 +3605,7 @@
       <c r="A56" s="31"/>
       <c r="B56" s="7"/>
       <c r="C56" s="7" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D56" s="29"/>
       <c r="E56" s="28"/>
@@ -3630,7 +3630,7 @@
       <c r="A57" s="31"/>
       <c r="B57" s="7"/>
       <c r="C57" s="7" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D57" s="29"/>
       <c r="E57" s="28"/>
@@ -3655,7 +3655,7 @@
       <c r="A58" s="31"/>
       <c r="B58" s="7"/>
       <c r="C58" s="7" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D58" s="29"/>
       <c r="E58" s="28"/>
@@ -3680,7 +3680,7 @@
       <c r="A59" s="31"/>
       <c r="B59" s="7"/>
       <c r="C59" s="7" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D59" s="29"/>
       <c r="E59" s="28"/>
@@ -3705,7 +3705,7 @@
       <c r="A60" s="31"/>
       <c r="B60" s="7"/>
       <c r="C60" s="7" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="D60" s="29"/>
       <c r="E60" s="28"/>
@@ -3730,7 +3730,7 @@
       <c r="A61" s="31"/>
       <c r="B61" s="7"/>
       <c r="C61" s="6" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="D61" s="29"/>
       <c r="E61" s="28"/>
@@ -3754,7 +3754,7 @@
     <row r="62" spans="1:11" ht="18.75" customHeight="1">
       <c r="A62" s="31"/>
       <c r="B62" s="2" t="s">
-        <v>345</v>
+        <v>349</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>6</v>
@@ -3860,10 +3860,10 @@
       <c r="A66" s="31"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
       <c r="D66" s="29" t="s">
-        <v>239</v>
+        <v>246</v>
       </c>
       <c r="E66" s="28"/>
       <c r="G66" s="40">
@@ -3887,7 +3887,7 @@
       <c r="A67" s="31"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D67" s="29"/>
       <c r="E67" s="28"/>
@@ -3912,7 +3912,7 @@
       <c r="A68" s="31"/>
       <c r="B68" s="3"/>
       <c r="C68" s="3" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D68" s="29"/>
       <c r="E68" s="28"/>
@@ -3937,7 +3937,7 @@
       <c r="A69" s="31"/>
       <c r="B69" s="4"/>
       <c r="C69" s="4" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="D69" s="29"/>
       <c r="E69" s="28"/>
@@ -3961,7 +3961,7 @@
     <row r="70" spans="1:11" ht="18.75" customHeight="1">
       <c r="A70" s="31"/>
       <c r="B70" s="5" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c r="C70" s="5" t="s">
         <v>8</v>
@@ -4017,7 +4017,7 @@
       <c r="A72" s="31"/>
       <c r="B72" s="7"/>
       <c r="C72" s="7" t="s">
-        <v>249</v>
+        <v>256</v>
       </c>
       <c r="D72" s="29"/>
       <c r="E72" s="28"/>
@@ -4042,7 +4042,7 @@
       <c r="A73" s="31"/>
       <c r="B73" s="7"/>
       <c r="C73" s="7" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="D73" s="29"/>
       <c r="E73" s="28"/>
@@ -4067,7 +4067,7 @@
       <c r="A74" s="31"/>
       <c r="B74" s="7"/>
       <c r="C74" s="7" t="s">
-        <v>250</v>
+        <v>257</v>
       </c>
       <c r="D74" s="29"/>
       <c r="E74" s="28"/>
@@ -4092,7 +4092,7 @@
       <c r="A75" s="31"/>
       <c r="B75" s="7"/>
       <c r="C75" s="7" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D75" s="29"/>
       <c r="E75" s="28"/>
@@ -4117,7 +4117,7 @@
       <c r="A76" s="31"/>
       <c r="B76" s="7"/>
       <c r="C76" s="7" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D76" s="29"/>
       <c r="E76" s="28"/>
@@ -4142,7 +4142,7 @@
       <c r="A77" s="31"/>
       <c r="B77" s="7"/>
       <c r="C77" s="7" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D77" s="29"/>
       <c r="E77" s="28"/>
@@ -4167,10 +4167,10 @@
       <c r="A78" s="31"/>
       <c r="B78" s="7"/>
       <c r="C78" s="7" t="s">
-        <v>251</v>
+        <v>258</v>
       </c>
       <c r="D78" s="29" t="s">
-        <v>256</v>
+        <v>263</v>
       </c>
       <c r="E78" s="28"/>
       <c r="G78" s="40">
@@ -4194,10 +4194,10 @@
       <c r="A79" s="31"/>
       <c r="B79" s="7"/>
       <c r="C79" s="7" t="s">
-        <v>252</v>
+        <v>259</v>
       </c>
       <c r="D79" s="29" t="s">
-        <v>257</v>
+        <v>264</v>
       </c>
       <c r="E79" s="28"/>
       <c r="G79" s="40">
@@ -4221,7 +4221,7 @@
       <c r="A80" s="31"/>
       <c r="B80" s="7"/>
       <c r="C80" s="7" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D80" s="29"/>
       <c r="E80" s="28"/>
@@ -4246,7 +4246,7 @@
       <c r="A81" s="31"/>
       <c r="B81" s="7"/>
       <c r="C81" s="7" t="s">
-        <v>253</v>
+        <v>260</v>
       </c>
       <c r="D81" s="29"/>
       <c r="E81" s="28"/>
@@ -4271,7 +4271,7 @@
       <c r="A82" s="31"/>
       <c r="B82" s="7"/>
       <c r="C82" s="7" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D82" s="29"/>
       <c r="E82" s="28"/>
@@ -4296,7 +4296,7 @@
       <c r="A83" s="31"/>
       <c r="B83" s="7"/>
       <c r="C83" s="7" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D83" s="29"/>
       <c r="E83" s="28"/>
@@ -4321,7 +4321,7 @@
       <c r="A84" s="31"/>
       <c r="B84" s="7"/>
       <c r="C84" s="7" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D84" s="29"/>
       <c r="E84" s="28"/>
@@ -4346,7 +4346,7 @@
       <c r="A85" s="31"/>
       <c r="B85" s="7"/>
       <c r="C85" s="7" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D85" s="29"/>
       <c r="E85" s="28"/>
@@ -4371,7 +4371,7 @@
       <c r="A86" s="31"/>
       <c r="B86" s="7"/>
       <c r="C86" s="7" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="D86" s="29"/>
       <c r="E86" s="28"/>
@@ -4396,7 +4396,7 @@
       <c r="A87" s="31"/>
       <c r="B87" s="6"/>
       <c r="C87" s="6" t="s">
-        <v>254</v>
+        <v>261</v>
       </c>
       <c r="D87" s="29"/>
       <c r="E87" s="28"/>
@@ -4420,10 +4420,10 @@
     <row r="88" spans="1:11" ht="18.75" customHeight="1">
       <c r="A88" s="31"/>
       <c r="B88" s="2" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="D88" s="29"/>
       <c r="E88" s="28"/>
@@ -4451,7 +4451,7 @@
       <c r="A89" s="31"/>
       <c r="B89" s="3"/>
       <c r="C89" s="3" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="D89" s="29"/>
       <c r="E89" s="28"/>
@@ -4476,7 +4476,7 @@
       <c r="A90" s="31"/>
       <c r="B90" s="3"/>
       <c r="C90" s="3" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="D90" s="29"/>
       <c r="E90" s="28"/>
@@ -4501,7 +4501,7 @@
       <c r="A91" s="31"/>
       <c r="B91" s="3"/>
       <c r="C91" s="3" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="D91" s="29"/>
       <c r="E91" s="28"/>
@@ -4526,7 +4526,7 @@
       <c r="A92" s="31"/>
       <c r="B92" s="3"/>
       <c r="C92" s="3" t="s">
-        <v>240</v>
+        <v>247</v>
       </c>
       <c r="D92" s="29"/>
       <c r="E92" s="28"/>
@@ -4550,7 +4550,7 @@
     <row r="93" spans="1:11" ht="18.75" customHeight="1">
       <c r="A93" s="31"/>
       <c r="B93" s="2" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C93" s="2" t="s">
         <v>33</v>
@@ -4581,10 +4581,10 @@
       <c r="A94" s="31"/>
       <c r="B94" s="3"/>
       <c r="C94" s="3" t="s">
-        <v>241</v>
+        <v>248</v>
       </c>
       <c r="D94" s="29" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="E94" s="28"/>
       <c r="G94" s="40">
@@ -4608,7 +4608,7 @@
       <c r="A95" s="31"/>
       <c r="B95" s="3"/>
       <c r="C95" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D95" s="29"/>
       <c r="E95" s="28"/>
@@ -4633,7 +4633,7 @@
       <c r="A96" s="31"/>
       <c r="B96" s="3"/>
       <c r="C96" s="3" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="D96" s="29"/>
       <c r="E96" s="28"/>
@@ -4658,7 +4658,7 @@
       <c r="A97" s="31"/>
       <c r="B97" s="3"/>
       <c r="C97" s="3" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="D97" s="29"/>
       <c r="E97" s="28"/>
@@ -4683,7 +4683,7 @@
       <c r="A98" s="31"/>
       <c r="B98" s="3"/>
       <c r="C98" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D98" s="29"/>
       <c r="E98" s="28"/>
@@ -4708,7 +4708,7 @@
       <c r="A99" s="31"/>
       <c r="B99" s="3"/>
       <c r="C99" s="3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D99" s="29"/>
       <c r="E99" s="28"/>
@@ -4733,7 +4733,7 @@
       <c r="A100" s="31"/>
       <c r="B100" s="3"/>
       <c r="C100" s="3" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="D100" s="29"/>
       <c r="E100" s="28"/>
@@ -4758,7 +4758,7 @@
       <c r="A101" s="31"/>
       <c r="B101" s="3"/>
       <c r="C101" s="3" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="D101" s="29"/>
       <c r="E101" s="28"/>
@@ -4783,7 +4783,7 @@
       <c r="A102" s="31"/>
       <c r="B102" s="3"/>
       <c r="C102" s="3" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="D102" s="29"/>
       <c r="E102" s="28"/>
@@ -4808,7 +4808,7 @@
       <c r="A103" s="31"/>
       <c r="B103" s="3"/>
       <c r="C103" s="3" t="s">
-        <v>261</v>
+        <v>268</v>
       </c>
       <c r="D103" s="29"/>
       <c r="E103" s="28"/>
@@ -4936,7 +4936,7 @@
       <c r="A108" s="31"/>
       <c r="B108" s="3"/>
       <c r="C108" s="3" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="D108" s="29"/>
       <c r="E108" s="28"/>
@@ -4961,7 +4961,7 @@
       <c r="A109" s="31"/>
       <c r="B109" s="3"/>
       <c r="C109" s="2" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="D109" s="29"/>
       <c r="E109" s="28"/>
@@ -4989,10 +4989,10 @@
       <c r="A110" s="31"/>
       <c r="B110" s="3"/>
       <c r="C110" s="3" t="s">
-        <v>262</v>
+        <v>269</v>
       </c>
       <c r="D110" s="29" t="s">
-        <v>263</v>
+        <v>270</v>
       </c>
       <c r="E110" s="28"/>
       <c r="G110" s="40">
@@ -5091,7 +5091,7 @@
       <c r="A114" s="31"/>
       <c r="B114" s="3"/>
       <c r="C114" s="3" t="s">
-        <v>264</v>
+        <v>271</v>
       </c>
       <c r="D114" s="29"/>
       <c r="E114" s="28"/>
@@ -5116,10 +5116,10 @@
       <c r="A115" s="31"/>
       <c r="B115" s="3"/>
       <c r="C115" s="3" t="s">
-        <v>265</v>
+        <v>272</v>
       </c>
       <c r="D115" s="29" t="s">
-        <v>266</v>
+        <v>273</v>
       </c>
       <c r="E115" s="28"/>
       <c r="G115" s="40">
@@ -5143,7 +5143,7 @@
       <c r="A116" s="31"/>
       <c r="B116" s="3"/>
       <c r="C116" s="3" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="D116" s="29"/>
       <c r="E116" s="28"/>
@@ -5168,7 +5168,7 @@
       <c r="A117" s="31"/>
       <c r="B117" s="3"/>
       <c r="C117" s="3" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="D117" s="29"/>
       <c r="E117" s="28"/>
@@ -5193,7 +5193,7 @@
       <c r="A118" s="31"/>
       <c r="B118" s="3"/>
       <c r="C118" s="3" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="D118" s="29"/>
       <c r="E118" s="28"/>
@@ -5218,7 +5218,7 @@
       <c r="A119" s="31"/>
       <c r="B119" s="3"/>
       <c r="C119" s="3" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="D119" s="29"/>
       <c r="E119" s="28"/>
@@ -5242,13 +5242,13 @@
     <row r="120" spans="1:11" ht="18.75" customHeight="1">
       <c r="A120" s="31"/>
       <c r="B120" s="2" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>267</v>
+        <v>274</v>
       </c>
       <c r="D120" s="29" t="s">
-        <v>444</v>
+        <v>447</v>
       </c>
       <c r="E120" s="28"/>
       <c r="G120" s="40">
@@ -5275,7 +5275,7 @@
       <c r="A121" s="31"/>
       <c r="B121" s="3"/>
       <c r="C121" s="3" t="s">
-        <v>268</v>
+        <v>275</v>
       </c>
       <c r="D121" s="29"/>
       <c r="E121" s="28"/>
@@ -5300,7 +5300,7 @@
       <c r="A122" s="31"/>
       <c r="B122" s="3"/>
       <c r="C122" s="3" t="s">
-        <v>269</v>
+        <v>276</v>
       </c>
       <c r="D122" s="29"/>
       <c r="E122" s="28"/>
@@ -5325,7 +5325,7 @@
       <c r="A123" s="31"/>
       <c r="B123" s="3"/>
       <c r="C123" s="3" t="s">
-        <v>270</v>
+        <v>277</v>
       </c>
       <c r="D123" s="29"/>
       <c r="E123" s="28"/>
@@ -5350,7 +5350,7 @@
       <c r="A124" s="31"/>
       <c r="B124" s="3"/>
       <c r="C124" s="3" t="s">
-        <v>271</v>
+        <v>278</v>
       </c>
       <c r="D124" s="29"/>
       <c r="E124" s="28"/>
@@ -5375,7 +5375,7 @@
       <c r="A125" s="31"/>
       <c r="B125" s="3"/>
       <c r="C125" s="3" t="s">
-        <v>272</v>
+        <v>279</v>
       </c>
       <c r="D125" s="29"/>
       <c r="E125" s="28"/>
@@ -5400,7 +5400,7 @@
       <c r="A126" s="31"/>
       <c r="B126" s="3"/>
       <c r="C126" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D126" s="29"/>
       <c r="E126" s="28"/>
@@ -5453,7 +5453,7 @@
       <c r="A128" s="31"/>
       <c r="B128" s="3"/>
       <c r="C128" s="3" t="s">
-        <v>273</v>
+        <v>280</v>
       </c>
       <c r="D128" s="29"/>
       <c r="E128" s="28"/>
@@ -5503,7 +5503,7 @@
       <c r="A130" s="31"/>
       <c r="B130" s="3"/>
       <c r="C130" s="4" t="s">
-        <v>274</v>
+        <v>281</v>
       </c>
       <c r="D130" s="29"/>
       <c r="E130" s="28"/>
@@ -5528,10 +5528,10 @@
       <c r="A131" s="31"/>
       <c r="B131" s="3"/>
       <c r="C131" s="3" t="s">
-        <v>275</v>
+        <v>282</v>
       </c>
       <c r="D131" s="29" t="s">
-        <v>276</v>
+        <v>283</v>
       </c>
       <c r="E131" s="28"/>
       <c r="G131" s="40">
@@ -5558,10 +5558,10 @@
       <c r="A132" s="31"/>
       <c r="B132" s="3"/>
       <c r="C132" s="3" t="s">
-        <v>279</v>
+        <v>286</v>
       </c>
       <c r="D132" s="29" t="s">
-        <v>277</v>
+        <v>284</v>
       </c>
       <c r="E132" s="28"/>
       <c r="G132" s="40">
@@ -5585,10 +5585,10 @@
       <c r="A133" s="31"/>
       <c r="B133" s="3"/>
       <c r="C133" s="3" t="s">
-        <v>280</v>
+        <v>287</v>
       </c>
       <c r="D133" s="29" t="s">
-        <v>278</v>
+        <v>285</v>
       </c>
       <c r="E133" s="28"/>
       <c r="G133" s="40">
@@ -5612,10 +5612,10 @@
       <c r="A134" s="31"/>
       <c r="B134" s="3"/>
       <c r="C134" s="3" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="D134" s="29" t="s">
-        <v>282</v>
+        <v>289</v>
       </c>
       <c r="E134" s="28"/>
       <c r="G134" s="40">
@@ -5639,7 +5639,7 @@
       <c r="A135" s="31"/>
       <c r="B135" s="3"/>
       <c r="C135" s="3" t="s">
-        <v>283</v>
+        <v>290</v>
       </c>
       <c r="D135" s="29"/>
       <c r="E135" s="28"/>
@@ -5664,7 +5664,7 @@
       <c r="A136" s="31"/>
       <c r="B136" s="3"/>
       <c r="C136" s="3" t="s">
-        <v>284</v>
+        <v>291</v>
       </c>
       <c r="D136" s="29"/>
       <c r="E136" s="28"/>
@@ -5689,7 +5689,7 @@
       <c r="A137" s="31"/>
       <c r="B137" s="3"/>
       <c r="C137" s="3" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D137" s="29"/>
       <c r="E137" s="28"/>
@@ -5714,7 +5714,7 @@
       <c r="A138" s="31"/>
       <c r="B138" s="3"/>
       <c r="C138" s="3" t="s">
-        <v>285</v>
+        <v>292</v>
       </c>
       <c r="D138" s="29"/>
       <c r="E138" s="28"/>
@@ -5739,7 +5739,7 @@
       <c r="A139" s="31"/>
       <c r="B139" s="3"/>
       <c r="C139" s="3" t="s">
-        <v>286</v>
+        <v>293</v>
       </c>
       <c r="D139" s="29"/>
       <c r="E139" s="28"/>
@@ -5764,7 +5764,7 @@
       <c r="A140" s="31"/>
       <c r="B140" s="3"/>
       <c r="C140" s="3" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D140" s="29"/>
       <c r="E140" s="28"/>
@@ -5789,7 +5789,7 @@
       <c r="A141" s="31"/>
       <c r="B141" s="3"/>
       <c r="C141" s="3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D141" s="29"/>
       <c r="E141" s="28"/>
@@ -5814,7 +5814,7 @@
       <c r="A142" s="31"/>
       <c r="B142" s="3"/>
       <c r="C142" s="3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D142" s="29"/>
       <c r="E142" s="28"/>
@@ -5839,7 +5839,7 @@
       <c r="A143" s="31"/>
       <c r="B143" s="3"/>
       <c r="C143" s="3" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D143" s="29"/>
       <c r="E143" s="28"/>
@@ -5864,7 +5864,7 @@
       <c r="A144" s="31"/>
       <c r="B144" s="4"/>
       <c r="C144" s="3" t="s">
-        <v>287</v>
+        <v>294</v>
       </c>
       <c r="D144" s="29"/>
       <c r="E144" s="28"/>
@@ -5888,13 +5888,13 @@
     <row r="145" spans="1:11" ht="18.75" customHeight="1">
       <c r="A145" s="31"/>
       <c r="B145" s="2" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>288</v>
+        <v>295</v>
       </c>
       <c r="D145" s="29" t="s">
-        <v>289</v>
+        <v>296</v>
       </c>
       <c r="E145" s="28"/>
       <c r="G145" s="40">
@@ -5921,7 +5921,7 @@
       <c r="A146" s="31"/>
       <c r="B146" s="20"/>
       <c r="C146" s="3" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D146" s="29"/>
       <c r="E146" s="28"/>
@@ -5946,7 +5946,7 @@
       <c r="A147" s="31"/>
       <c r="B147" s="20"/>
       <c r="C147" s="3" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D147" s="29"/>
       <c r="E147" s="28"/>
@@ -5996,10 +5996,10 @@
       <c r="A149" s="31"/>
       <c r="B149" s="20"/>
       <c r="C149" s="3" t="s">
-        <v>290</v>
+        <v>297</v>
       </c>
       <c r="D149" s="29" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="E149" s="28"/>
       <c r="G149" s="40">
@@ -6023,7 +6023,7 @@
       <c r="A150" s="31"/>
       <c r="B150" s="20"/>
       <c r="C150" s="3" t="s">
-        <v>292</v>
+        <v>299</v>
       </c>
       <c r="D150" s="29"/>
       <c r="E150" s="28"/>
@@ -6047,7 +6047,7 @@
     <row r="151" spans="1:11" ht="18.75" customHeight="1">
       <c r="A151" s="31"/>
       <c r="B151" s="2" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C151" s="2" t="s">
         <v>32</v>
@@ -6078,7 +6078,7 @@
       <c r="A152" s="31"/>
       <c r="B152" s="3"/>
       <c r="C152" s="3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D152" s="29"/>
       <c r="E152" s="28"/>
@@ -6128,7 +6128,7 @@
       <c r="A154" s="31"/>
       <c r="B154" s="3"/>
       <c r="C154" s="3" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D154" s="29"/>
       <c r="E154" s="28"/>
@@ -6153,7 +6153,7 @@
       <c r="A155" s="31"/>
       <c r="B155" s="4"/>
       <c r="C155" s="4" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="D155" s="29"/>
       <c r="E155" s="28"/>
@@ -6177,10 +6177,10 @@
     <row r="156" spans="1:11" ht="18.75" customHeight="1">
       <c r="A156" s="31"/>
       <c r="B156" s="5" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C156" s="5" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D156" s="29"/>
       <c r="E156" s="28"/>
@@ -6208,7 +6208,7 @@
       <c r="A157" s="31"/>
       <c r="B157" s="7"/>
       <c r="C157" s="7" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
       <c r="D157" s="29"/>
       <c r="E157" s="28"/>
@@ -6233,7 +6233,7 @@
       <c r="A158" s="31"/>
       <c r="B158" s="7"/>
       <c r="C158" s="7" t="s">
-        <v>293</v>
+        <v>300</v>
       </c>
       <c r="D158" s="29"/>
       <c r="E158" s="28"/>
@@ -6258,7 +6258,7 @@
       <c r="A159" s="31"/>
       <c r="B159" s="7"/>
       <c r="C159" s="7" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D159" s="29"/>
       <c r="E159" s="28"/>
@@ -6283,7 +6283,7 @@
       <c r="A160" s="31"/>
       <c r="B160" s="7"/>
       <c r="C160" s="7" t="s">
-        <v>295</v>
+        <v>302</v>
       </c>
       <c r="D160" s="29"/>
       <c r="E160" s="28"/>
@@ -6358,7 +6358,7 @@
       <c r="A163" s="31"/>
       <c r="B163" s="7"/>
       <c r="C163" s="7" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D163" s="29"/>
       <c r="E163" s="28"/>
@@ -6383,7 +6383,7 @@
       <c r="A164" s="31"/>
       <c r="B164" s="7"/>
       <c r="C164" s="7" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D164" s="29"/>
       <c r="E164" s="28"/>
@@ -6408,7 +6408,7 @@
       <c r="A165" s="31"/>
       <c r="B165" s="7"/>
       <c r="C165" s="7" t="s">
-        <v>296</v>
+        <v>303</v>
       </c>
       <c r="D165" s="29"/>
       <c r="E165" s="28"/>
@@ -6432,10 +6432,10 @@
     <row r="166" spans="1:11" ht="18.75" customHeight="1">
       <c r="A166" s="31"/>
       <c r="B166" s="5" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C166" s="5" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D166" s="29"/>
       <c r="E166" s="28"/>
@@ -6463,7 +6463,7 @@
       <c r="A167" s="31"/>
       <c r="B167" s="7"/>
       <c r="C167" s="7" t="s">
-        <v>297</v>
+        <v>304</v>
       </c>
       <c r="D167" s="29"/>
       <c r="E167" s="28"/>
@@ -6488,10 +6488,10 @@
       <c r="A168" s="31"/>
       <c r="B168" s="7"/>
       <c r="C168" s="7" t="s">
-        <v>298</v>
+        <v>305</v>
       </c>
       <c r="D168" s="29" t="s">
-        <v>299</v>
+        <v>306</v>
       </c>
       <c r="E168" s="28"/>
       <c r="G168" s="40">
@@ -6515,7 +6515,7 @@
       <c r="A169" s="31"/>
       <c r="B169" s="7"/>
       <c r="C169" s="7" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D169" s="29"/>
       <c r="E169" s="28"/>
@@ -6540,7 +6540,7 @@
       <c r="A170" s="31"/>
       <c r="B170" s="7"/>
       <c r="C170" s="7" t="s">
-        <v>300</v>
+        <v>307</v>
       </c>
       <c r="D170" s="29"/>
       <c r="E170" s="28"/>
@@ -6564,10 +6564,10 @@
     <row r="171" spans="1:11" ht="18.75" customHeight="1" thickBot="1">
       <c r="A171" s="31"/>
       <c r="B171" s="5" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C171" s="5" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D171" s="29"/>
       <c r="E171" s="28"/>
@@ -6594,10 +6594,10 @@
     <row r="172" spans="1:11" ht="18.75" customHeight="1">
       <c r="A172" s="31"/>
       <c r="B172" s="2" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D172" s="29"/>
       <c r="E172" s="28"/>
@@ -6625,7 +6625,7 @@
       <c r="A173" s="31"/>
       <c r="B173" s="3"/>
       <c r="C173" s="3" t="s">
-        <v>301</v>
+        <v>308</v>
       </c>
       <c r="D173" s="29"/>
       <c r="E173" s="28"/>
@@ -6650,10 +6650,10 @@
       <c r="A174" s="31"/>
       <c r="B174" s="3"/>
       <c r="C174" s="3" t="s">
-        <v>302</v>
+        <v>309</v>
       </c>
       <c r="D174" s="29" t="s">
-        <v>303</v>
+        <v>310</v>
       </c>
       <c r="E174" s="28"/>
       <c r="G174" s="40">
@@ -6677,7 +6677,7 @@
       <c r="A175" s="31"/>
       <c r="B175" s="3"/>
       <c r="C175" s="3" t="s">
-        <v>304</v>
+        <v>456</v>
       </c>
       <c r="D175" s="29"/>
       <c r="E175" s="28"/>
@@ -6702,7 +6702,7 @@
       <c r="A176" s="31"/>
       <c r="B176" s="3"/>
       <c r="C176" s="3" t="s">
-        <v>305</v>
+        <v>311</v>
       </c>
       <c r="D176" s="29"/>
       <c r="E176" s="28"/>
@@ -6726,10 +6726,10 @@
     <row r="177" spans="1:11" ht="18.75" customHeight="1">
       <c r="A177" s="31"/>
       <c r="B177" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D177" s="29"/>
       <c r="E177" s="28"/>
@@ -6757,7 +6757,7 @@
       <c r="A178" s="31"/>
       <c r="B178" s="3"/>
       <c r="C178" s="3" t="s">
-        <v>306</v>
+        <v>312</v>
       </c>
       <c r="D178" s="29"/>
       <c r="E178" s="28"/>
@@ -6782,7 +6782,7 @@
       <c r="A179" s="31"/>
       <c r="B179" s="3"/>
       <c r="C179" s="3" t="s">
-        <v>307</v>
+        <v>313</v>
       </c>
       <c r="D179" s="29"/>
       <c r="E179" s="28"/>
@@ -6807,7 +6807,7 @@
       <c r="A180" s="31"/>
       <c r="B180" s="3"/>
       <c r="C180" s="3" t="s">
-        <v>308</v>
+        <v>314</v>
       </c>
       <c r="D180" s="29"/>
       <c r="E180" s="28"/>
@@ -6832,7 +6832,7 @@
       <c r="A181" s="31"/>
       <c r="B181" s="3"/>
       <c r="C181" s="3" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="D181" s="29"/>
       <c r="E181" s="28"/>
@@ -6857,7 +6857,7 @@
       <c r="A182" s="31"/>
       <c r="B182" s="3"/>
       <c r="C182" s="3" t="s">
-        <v>309</v>
+        <v>315</v>
       </c>
       <c r="D182" s="29"/>
       <c r="E182" s="28"/>
@@ -6882,7 +6882,7 @@
       <c r="A183" s="31"/>
       <c r="B183" s="3"/>
       <c r="C183" s="4" t="s">
-        <v>310</v>
+        <v>316</v>
       </c>
       <c r="D183" s="29"/>
       <c r="E183" s="28"/>
@@ -6909,7 +6909,7 @@
         <v>15</v>
       </c>
       <c r="C184" s="5" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D184" s="29"/>
       <c r="E184" s="28"/>
@@ -6987,10 +6987,10 @@
       <c r="A187" s="31"/>
       <c r="B187" s="7"/>
       <c r="C187" s="7" t="s">
-        <v>311</v>
+        <v>317</v>
       </c>
       <c r="D187" s="29" t="s">
-        <v>312</v>
+        <v>318</v>
       </c>
       <c r="E187" s="28"/>
       <c r="G187" s="40">
@@ -7014,7 +7014,7 @@
       <c r="A188" s="31"/>
       <c r="B188" s="7"/>
       <c r="C188" s="7" t="s">
-        <v>313</v>
+        <v>319</v>
       </c>
       <c r="D188" s="29"/>
       <c r="E188" s="28"/>
@@ -7039,10 +7039,10 @@
       <c r="A189" s="31"/>
       <c r="B189" s="7"/>
       <c r="C189" s="7" t="s">
-        <v>314</v>
+        <v>320</v>
       </c>
       <c r="D189" s="29" t="s">
-        <v>315</v>
+        <v>321</v>
       </c>
       <c r="E189" s="28"/>
       <c r="G189" s="40">
@@ -7066,7 +7066,7 @@
       <c r="A190" s="31"/>
       <c r="B190" s="7"/>
       <c r="C190" s="7" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D190" s="29"/>
       <c r="E190" s="28"/>
@@ -7091,10 +7091,10 @@
       <c r="A191" s="31"/>
       <c r="B191" s="7"/>
       <c r="C191" s="7" t="s">
-        <v>316</v>
+        <v>322</v>
       </c>
       <c r="D191" s="29" t="s">
-        <v>317</v>
+        <v>323</v>
       </c>
       <c r="E191" s="28"/>
       <c r="G191" s="40">
@@ -7118,7 +7118,7 @@
       <c r="A192" s="31"/>
       <c r="B192" s="6"/>
       <c r="C192" s="6" t="s">
-        <v>318</v>
+        <v>324</v>
       </c>
       <c r="D192" s="29"/>
       <c r="E192" s="28"/>
@@ -7142,7 +7142,7 @@
     <row r="193" spans="1:11" ht="18.75" customHeight="1">
       <c r="A193" s="31"/>
       <c r="B193" s="21" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C193" s="2" t="s">
         <v>12</v>
@@ -7173,7 +7173,7 @@
       <c r="A194" s="31"/>
       <c r="B194" s="22"/>
       <c r="C194" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D194" s="29"/>
       <c r="E194" s="28"/>
@@ -7223,7 +7223,7 @@
       <c r="A196" s="31"/>
       <c r="B196" s="3"/>
       <c r="C196" s="3" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D196" s="29"/>
       <c r="E196" s="28"/>
@@ -7251,7 +7251,7 @@
       <c r="A197" s="31"/>
       <c r="B197" s="3"/>
       <c r="C197" s="3" t="s">
-        <v>319</v>
+        <v>325</v>
       </c>
       <c r="D197" s="29"/>
       <c r="E197" s="28"/>
@@ -7276,7 +7276,7 @@
       <c r="A198" s="31"/>
       <c r="B198" s="3"/>
       <c r="C198" s="3" t="s">
-        <v>320</v>
+        <v>326</v>
       </c>
       <c r="D198" s="29"/>
       <c r="E198" s="28"/>
@@ -7301,7 +7301,7 @@
       <c r="A199" s="31"/>
       <c r="B199" s="3"/>
       <c r="C199" s="3" t="s">
-        <v>321</v>
+        <v>327</v>
       </c>
       <c r="D199" s="29"/>
       <c r="E199" s="28"/>
@@ -7326,7 +7326,7 @@
       <c r="A200" s="31"/>
       <c r="B200" s="3"/>
       <c r="C200" s="3" t="s">
-        <v>322</v>
+        <v>328</v>
       </c>
       <c r="D200" s="29"/>
       <c r="E200" s="28"/>
@@ -7351,7 +7351,7 @@
       <c r="A201" s="31"/>
       <c r="B201" s="3"/>
       <c r="C201" s="3" t="s">
-        <v>323</v>
+        <v>329</v>
       </c>
       <c r="D201" s="29"/>
       <c r="E201" s="28"/>
@@ -7376,7 +7376,7 @@
       <c r="A202" s="31"/>
       <c r="B202" s="3"/>
       <c r="C202" s="3" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="D202" s="29"/>
       <c r="E202" s="28"/>
@@ -7401,10 +7401,10 @@
       <c r="A203" s="31"/>
       <c r="B203" s="3"/>
       <c r="C203" s="3" t="s">
-        <v>324</v>
+        <v>330</v>
       </c>
       <c r="D203" s="29" t="s">
-        <v>325</v>
+        <v>331</v>
       </c>
       <c r="E203" s="28"/>
       <c r="G203" s="40">
@@ -7428,10 +7428,10 @@
       <c r="A204" s="31"/>
       <c r="B204" s="3"/>
       <c r="C204" s="3" t="s">
-        <v>326</v>
+        <v>332</v>
       </c>
       <c r="D204" s="29" t="s">
-        <v>327</v>
+        <v>333</v>
       </c>
       <c r="E204" s="28"/>
       <c r="G204" s="40">
@@ -7455,10 +7455,10 @@
       <c r="A205" s="31"/>
       <c r="B205" s="3"/>
       <c r="C205" s="3" t="s">
-        <v>328</v>
+        <v>334</v>
       </c>
       <c r="D205" s="29" t="s">
-        <v>329</v>
+        <v>335</v>
       </c>
       <c r="E205" s="28"/>
       <c r="G205" s="40">
@@ -7482,7 +7482,7 @@
       <c r="A206" s="31"/>
       <c r="B206" s="3"/>
       <c r="C206" s="3" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="D206" s="29"/>
       <c r="E206" s="28"/>
@@ -7507,7 +7507,7 @@
       <c r="A207" s="31"/>
       <c r="B207" s="3"/>
       <c r="C207" s="4" t="s">
-        <v>330</v>
+        <v>336</v>
       </c>
       <c r="D207" s="29"/>
       <c r="E207" s="28"/>
@@ -7531,7 +7531,7 @@
     <row r="208" spans="1:11" ht="18.75" customHeight="1">
       <c r="A208" s="31"/>
       <c r="B208" s="21" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C208" s="2" t="s">
         <v>13</v>
@@ -7562,7 +7562,7 @@
       <c r="A209" s="31"/>
       <c r="B209" s="27"/>
       <c r="C209" s="3" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="D209" s="29"/>
       <c r="E209" s="28"/>
@@ -7587,7 +7587,7 @@
       <c r="A210" s="31"/>
       <c r="B210" s="3"/>
       <c r="C210" s="3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D210" s="29"/>
       <c r="E210" s="28"/>
@@ -7612,10 +7612,10 @@
       <c r="A211" s="31"/>
       <c r="B211" s="3"/>
       <c r="C211" s="3" t="s">
-        <v>331</v>
+        <v>337</v>
       </c>
       <c r="D211" s="29" t="s">
-        <v>332</v>
+        <v>338</v>
       </c>
       <c r="E211" s="28"/>
       <c r="G211" s="40">
@@ -7639,10 +7639,10 @@
       <c r="A212" s="31"/>
       <c r="B212" s="3"/>
       <c r="C212" s="3" t="s">
-        <v>333</v>
+        <v>339</v>
       </c>
       <c r="D212" s="29" t="s">
-        <v>334</v>
+        <v>340</v>
       </c>
       <c r="E212" s="28"/>
       <c r="G212" s="40">
@@ -7666,10 +7666,10 @@
       <c r="A213" s="31"/>
       <c r="B213" s="3"/>
       <c r="C213" s="3" t="s">
-        <v>335</v>
+        <v>341</v>
       </c>
       <c r="D213" s="29" t="s">
-        <v>336</v>
+        <v>342</v>
       </c>
       <c r="E213" s="28"/>
       <c r="G213" s="40">
@@ -7693,7 +7693,7 @@
       <c r="A214" s="31"/>
       <c r="B214" s="3"/>
       <c r="C214" s="3" t="s">
-        <v>337</v>
+        <v>343</v>
       </c>
       <c r="D214" s="29"/>
       <c r="E214" s="28"/>
@@ -7718,7 +7718,7 @@
       <c r="A215" s="31"/>
       <c r="B215" s="3"/>
       <c r="C215" s="3" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="D215" s="29"/>
       <c r="E215" s="28"/>
@@ -7743,7 +7743,7 @@
       <c r="A216" s="31"/>
       <c r="B216" s="3"/>
       <c r="C216" s="3" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="D216" s="29"/>
       <c r="E216" s="28"/>
@@ -7768,7 +7768,7 @@
       <c r="A217" s="31"/>
       <c r="B217" s="3"/>
       <c r="C217" s="3" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="D217" s="29"/>
       <c r="E217" s="28"/>
@@ -7793,7 +7793,7 @@
       <c r="A218" s="31"/>
       <c r="B218" s="3"/>
       <c r="C218" s="3" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="D218" s="29"/>
       <c r="E218" s="28"/>
@@ -7818,7 +7818,7 @@
       <c r="A219" s="31"/>
       <c r="B219" s="3"/>
       <c r="C219" s="3" t="s">
-        <v>338</v>
+        <v>344</v>
       </c>
       <c r="D219" s="29"/>
       <c r="E219" s="28"/>
@@ -7845,7 +7845,7 @@
         <v>17</v>
       </c>
       <c r="C220" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D220" s="29"/>
       <c r="E220" s="28"/>
@@ -7873,7 +7873,7 @@
       <c r="A221" s="31"/>
       <c r="B221" s="3"/>
       <c r="C221" s="3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D221" s="29"/>
       <c r="E221" s="28"/>
@@ -7898,7 +7898,7 @@
       <c r="A222" s="31"/>
       <c r="B222" s="4"/>
       <c r="C222" s="4" t="s">
-        <v>339</v>
+        <v>345</v>
       </c>
       <c r="D222" s="29"/>
       <c r="E222" s="28"/>
@@ -7922,10 +7922,10 @@
     <row r="223" spans="1:11" ht="18.75" customHeight="1" thickBot="1">
       <c r="A223" s="31"/>
       <c r="B223" s="5" t="s">
-        <v>342</v>
+        <v>453</v>
       </c>
       <c r="C223" s="10" t="s">
-        <v>340</v>
+        <v>457</v>
       </c>
       <c r="D223" s="29"/>
       <c r="E223" s="28"/>
@@ -7952,10 +7952,10 @@
     <row r="224" spans="1:11" ht="18.75" customHeight="1" thickBot="1">
       <c r="A224" s="31"/>
       <c r="B224" s="11" t="s">
-        <v>343</v>
+        <v>347</v>
       </c>
       <c r="C224" s="11" t="s">
-        <v>341</v>
+        <v>346</v>
       </c>
       <c r="D224" s="29"/>
       <c r="E224" s="28"/>
@@ -7984,7 +7984,7 @@
         <v>18</v>
       </c>
       <c r="B225" s="12" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C225" s="12" t="s">
         <v>45</v>
@@ -8015,7 +8015,7 @@
       <c r="A226" s="33"/>
       <c r="B226" s="13"/>
       <c r="C226" s="13" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="D226" s="29"/>
       <c r="E226" s="28"/>
@@ -8040,7 +8040,7 @@
       <c r="A227" s="23"/>
       <c r="B227" s="13"/>
       <c r="C227" s="13" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
       <c r="D227" s="29"/>
       <c r="E227" s="28"/>
@@ -8065,7 +8065,7 @@
       <c r="A228" s="23"/>
       <c r="B228" s="13"/>
       <c r="C228" s="13" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="D228" s="29"/>
       <c r="E228" s="28"/>
@@ -8115,7 +8115,7 @@
       <c r="A230" s="23"/>
       <c r="B230" s="13"/>
       <c r="C230" s="13" t="s">
-        <v>354</v>
+        <v>358</v>
       </c>
       <c r="D230" s="29"/>
       <c r="E230" s="28"/>
@@ -8140,7 +8140,7 @@
       <c r="A231" s="23"/>
       <c r="B231" s="13"/>
       <c r="C231" s="14" t="s">
-        <v>349</v>
+        <v>353</v>
       </c>
       <c r="D231" s="29"/>
       <c r="E231" s="28"/>
@@ -8218,7 +8218,7 @@
       <c r="A234" s="23"/>
       <c r="B234" s="13"/>
       <c r="C234" s="17" t="s">
-        <v>353</v>
+        <v>357</v>
       </c>
       <c r="D234" s="29"/>
       <c r="E234" s="28"/>
@@ -8243,7 +8243,7 @@
       <c r="A235" s="23"/>
       <c r="B235" s="13"/>
       <c r="C235" s="17" t="s">
-        <v>351</v>
+        <v>355</v>
       </c>
       <c r="D235" s="29"/>
       <c r="E235" s="28"/>
@@ -8293,7 +8293,7 @@
       <c r="A237" s="23"/>
       <c r="B237" s="13"/>
       <c r="C237" s="17" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D237" s="29"/>
       <c r="E237" s="28"/>
@@ -8343,7 +8343,7 @@
       <c r="A239" s="23"/>
       <c r="B239" s="13"/>
       <c r="C239" s="17" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D239" s="29"/>
       <c r="E239" s="28"/>
@@ -8368,7 +8368,7 @@
       <c r="A240" s="23"/>
       <c r="B240" s="13"/>
       <c r="C240" s="17" t="s">
-        <v>352</v>
+        <v>356</v>
       </c>
       <c r="D240" s="29"/>
       <c r="E240" s="28"/>
@@ -8443,7 +8443,7 @@
       <c r="A243" s="23"/>
       <c r="B243" s="13"/>
       <c r="C243" s="17" t="s">
-        <v>355</v>
+        <v>359</v>
       </c>
       <c r="D243" s="29"/>
       <c r="E243" s="28"/>
@@ -8493,7 +8493,7 @@
       <c r="A245" s="23"/>
       <c r="B245" s="13"/>
       <c r="C245" s="18" t="s">
-        <v>356</v>
+        <v>360</v>
       </c>
       <c r="D245" s="29"/>
       <c r="E245" s="28"/>
@@ -8518,11 +8518,11 @@
       <c r="A246" s="23"/>
       <c r="B246" s="14"/>
       <c r="C246" s="15" t="s">
-        <v>358</v>
+        <v>362</v>
       </c>
       <c r="D246" s="29"/>
       <c r="E246" s="29" t="s">
-        <v>357</v>
+        <v>361</v>
       </c>
       <c r="G246" s="40">
         <f t="shared" si="12"/>
@@ -8547,14 +8547,14 @@
     <row r="247" spans="1:11" ht="18.75" customHeight="1">
       <c r="A247" s="23"/>
       <c r="B247" s="16" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C247" s="17" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="D247" s="29"/>
       <c r="E247" s="29" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="F247" s="29"/>
       <c r="G247" s="40">
@@ -8581,13 +8581,13 @@
       <c r="A248" s="23"/>
       <c r="B248" s="17"/>
       <c r="C248" s="17" t="s">
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="D248" s="29" t="s">
-        <v>445</v>
+        <v>448</v>
       </c>
       <c r="E248" s="29" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="F248" s="29"/>
       <c r="G248" s="40">
@@ -8611,11 +8611,11 @@
       <c r="A249" s="23"/>
       <c r="B249" s="17"/>
       <c r="C249" s="17" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="D249" s="29"/>
       <c r="E249" s="29" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="F249" s="29"/>
       <c r="G249" s="40">
@@ -8639,11 +8639,11 @@
       <c r="A250" s="23"/>
       <c r="B250" s="17"/>
       <c r="C250" s="17" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="D250" s="29"/>
       <c r="E250" s="29" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="F250" s="29"/>
       <c r="G250" s="40">
@@ -8667,11 +8667,11 @@
       <c r="A251" s="23"/>
       <c r="B251" s="17"/>
       <c r="C251" s="17" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="D251" s="29"/>
       <c r="E251" s="29" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="F251" s="29"/>
       <c r="G251" s="40">
@@ -8695,11 +8695,11 @@
       <c r="A252" s="23"/>
       <c r="B252" s="17"/>
       <c r="C252" s="17" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
       <c r="D252" s="29"/>
       <c r="E252" s="29" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="F252" s="29"/>
       <c r="G252" s="40">
@@ -8723,13 +8723,13 @@
       <c r="A253" s="23"/>
       <c r="B253" s="17"/>
       <c r="C253" s="18" t="s">
-        <v>362</v>
+        <v>366</v>
       </c>
       <c r="D253" s="29" t="s">
-        <v>363</v>
+        <v>367</v>
       </c>
       <c r="E253" s="29" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="F253" s="29"/>
       <c r="G253" s="40">
@@ -8753,11 +8753,11 @@
       <c r="A254" s="23"/>
       <c r="B254" s="17"/>
       <c r="C254" s="17" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="D254" s="29"/>
       <c r="E254" s="29" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="F254" s="29"/>
       <c r="G254" s="40">
@@ -8784,11 +8784,11 @@
       <c r="A255" s="23"/>
       <c r="B255" s="17"/>
       <c r="C255" s="18" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="D255" s="29"/>
       <c r="E255" s="29" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="F255" s="29"/>
       <c r="G255" s="40">
@@ -8812,11 +8812,11 @@
       <c r="A256" s="23"/>
       <c r="B256" s="24"/>
       <c r="C256" s="12" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D256" s="29"/>
       <c r="E256" s="29" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="F256" s="29"/>
       <c r="G256" s="40">
@@ -8843,11 +8843,11 @@
       <c r="A257" s="23"/>
       <c r="B257" s="24"/>
       <c r="C257" s="13" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D257" s="29"/>
       <c r="E257" s="29" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="F257" s="29"/>
       <c r="G257" s="40">
@@ -8871,11 +8871,11 @@
       <c r="A258" s="23"/>
       <c r="B258" s="24"/>
       <c r="C258" s="13" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D258" s="29"/>
       <c r="E258" s="29" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="F258" s="29"/>
       <c r="G258" s="40">
@@ -8899,11 +8899,11 @@
       <c r="A259" s="23"/>
       <c r="B259" s="24"/>
       <c r="C259" s="13" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="D259" s="29"/>
       <c r="E259" s="29" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="F259" s="29"/>
       <c r="G259" s="40">
@@ -8927,11 +8927,11 @@
       <c r="A260" s="23"/>
       <c r="B260" s="24"/>
       <c r="C260" s="13" t="s">
-        <v>364</v>
+        <v>368</v>
       </c>
       <c r="D260" s="29"/>
       <c r="E260" s="29" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="F260" s="29"/>
       <c r="G260" s="40">
@@ -8955,11 +8955,11 @@
       <c r="A261" s="23"/>
       <c r="B261" s="24"/>
       <c r="C261" s="13" t="s">
-        <v>365</v>
+        <v>369</v>
       </c>
       <c r="D261" s="29"/>
       <c r="E261" s="29" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="F261" s="29"/>
       <c r="G261" s="40">
@@ -8983,11 +8983,11 @@
       <c r="A262" s="23"/>
       <c r="B262" s="24"/>
       <c r="C262" s="13" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
       <c r="D262" s="29"/>
       <c r="E262" s="29" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="F262" s="29"/>
       <c r="G262" s="40">
@@ -9011,13 +9011,13 @@
       <c r="A263" s="23"/>
       <c r="B263" s="24"/>
       <c r="C263" s="13" t="s">
-        <v>367</v>
+        <v>371</v>
       </c>
       <c r="D263" s="29" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="E263" s="29" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="F263" s="29"/>
       <c r="G263" s="40">
@@ -9045,7 +9045,7 @@
       </c>
       <c r="D264" s="29"/>
       <c r="E264" s="29" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="F264" s="29"/>
       <c r="G264" s="40">
@@ -9073,7 +9073,7 @@
       </c>
       <c r="D265" s="29"/>
       <c r="E265" s="29" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="F265" s="29"/>
       <c r="G265" s="40">
@@ -9097,11 +9097,11 @@
       <c r="A266" s="23"/>
       <c r="B266" s="17"/>
       <c r="C266" s="12" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="D266" s="29"/>
       <c r="E266" s="29" t="s">
-        <v>359</v>
+        <v>363</v>
       </c>
       <c r="F266" s="29"/>
       <c r="G266" s="40">
@@ -9128,11 +9128,11 @@
       <c r="A267" s="23"/>
       <c r="B267" s="24"/>
       <c r="C267" s="13" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="D267" s="29"/>
       <c r="E267" s="29" t="s">
-        <v>359</v>
+        <v>363</v>
       </c>
       <c r="F267" s="29"/>
       <c r="G267" s="40">
@@ -9156,11 +9156,11 @@
       <c r="A268" s="23"/>
       <c r="B268" s="17"/>
       <c r="C268" s="13" t="s">
-        <v>371</v>
+        <v>375</v>
       </c>
       <c r="D268" s="29"/>
       <c r="E268" s="29" t="s">
-        <v>359</v>
+        <v>363</v>
       </c>
       <c r="F268" s="29"/>
       <c r="G268" s="40">
@@ -9184,11 +9184,11 @@
       <c r="A269" s="23"/>
       <c r="B269" s="17"/>
       <c r="C269" s="13" t="s">
-        <v>372</v>
+        <v>376</v>
       </c>
       <c r="D269" s="29"/>
       <c r="E269" s="29" t="s">
-        <v>359</v>
+        <v>363</v>
       </c>
       <c r="F269" s="29"/>
       <c r="G269" s="40">
@@ -9212,11 +9212,11 @@
       <c r="A270" s="23"/>
       <c r="B270" s="17"/>
       <c r="C270" s="13" t="s">
-        <v>373</v>
+        <v>377</v>
       </c>
       <c r="D270" s="29"/>
       <c r="E270" s="29" t="s">
-        <v>359</v>
+        <v>363</v>
       </c>
       <c r="F270" s="29"/>
       <c r="G270" s="40">
@@ -9240,11 +9240,11 @@
       <c r="A271" s="23"/>
       <c r="B271" s="17"/>
       <c r="C271" s="13" t="s">
-        <v>374</v>
+        <v>378</v>
       </c>
       <c r="D271" s="29"/>
       <c r="E271" s="29" t="s">
-        <v>359</v>
+        <v>363</v>
       </c>
       <c r="F271" s="29"/>
       <c r="G271" s="40">
@@ -9268,11 +9268,11 @@
       <c r="A272" s="23"/>
       <c r="B272" s="17"/>
       <c r="C272" s="13" t="s">
-        <v>375</v>
+        <v>379</v>
       </c>
       <c r="D272" s="29"/>
       <c r="E272" s="29" t="s">
-        <v>359</v>
+        <v>363</v>
       </c>
       <c r="F272" s="29"/>
       <c r="G272" s="40">
@@ -9296,11 +9296,11 @@
       <c r="A273" s="23"/>
       <c r="B273" s="18"/>
       <c r="C273" s="13" t="s">
-        <v>376</v>
+        <v>380</v>
       </c>
       <c r="D273" s="29"/>
       <c r="E273" s="29" t="s">
-        <v>359</v>
+        <v>363</v>
       </c>
       <c r="F273" s="29"/>
       <c r="G273" s="40">
@@ -9323,14 +9323,14 @@
     <row r="274" spans="1:11" ht="18.75" customHeight="1">
       <c r="A274" s="23"/>
       <c r="B274" s="12" t="s">
-        <v>419</v>
+        <v>423</v>
       </c>
       <c r="C274" s="12" t="s">
         <v>54</v>
       </c>
       <c r="D274" s="29"/>
       <c r="E274" s="29" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="F274" s="29"/>
       <c r="G274" s="40">
@@ -9361,7 +9361,7 @@
       </c>
       <c r="D275" s="29"/>
       <c r="E275" s="29" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="F275" s="29"/>
       <c r="G275" s="40">
@@ -9389,7 +9389,7 @@
       </c>
       <c r="D276" s="29"/>
       <c r="E276" s="29" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="F276" s="29"/>
       <c r="G276" s="40">
@@ -9417,7 +9417,7 @@
       </c>
       <c r="D277" s="29"/>
       <c r="E277" s="29" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="F277" s="29"/>
       <c r="G277" s="40">
@@ -9445,7 +9445,7 @@
       </c>
       <c r="D278" s="29"/>
       <c r="E278" s="29" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="F278" s="29"/>
       <c r="G278" s="40">
@@ -9469,11 +9469,11 @@
       <c r="A279" s="23"/>
       <c r="B279" s="13"/>
       <c r="C279" s="13" t="s">
-        <v>377</v>
+        <v>381</v>
       </c>
       <c r="D279" s="29"/>
       <c r="E279" s="29" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="F279" s="29"/>
       <c r="G279" s="40">
@@ -9501,7 +9501,7 @@
       </c>
       <c r="D280" s="29"/>
       <c r="E280" s="29" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="F280" s="29"/>
       <c r="G280" s="40">
@@ -9529,7 +9529,7 @@
       </c>
       <c r="D281" s="29"/>
       <c r="E281" s="29" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="F281" s="29"/>
       <c r="G281" s="40">
@@ -9557,7 +9557,7 @@
       </c>
       <c r="D282" s="29"/>
       <c r="E282" s="29" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="F282" s="29"/>
       <c r="G282" s="40">
@@ -9581,13 +9581,13 @@
       <c r="A283" s="23"/>
       <c r="B283" s="13"/>
       <c r="C283" s="13" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
       <c r="D283" s="29" t="s">
-        <v>447</v>
+        <v>450</v>
       </c>
       <c r="E283" s="29" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="F283" s="29"/>
       <c r="G283" s="40">
@@ -9611,11 +9611,11 @@
       <c r="A284" s="23"/>
       <c r="B284" s="13"/>
       <c r="C284" s="13" t="s">
-        <v>379</v>
+        <v>383</v>
       </c>
       <c r="D284" s="29"/>
       <c r="E284" s="29" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="F284" s="29"/>
       <c r="G284" s="40">
@@ -9639,11 +9639,11 @@
       <c r="A285" s="23"/>
       <c r="B285" s="13"/>
       <c r="C285" s="14" t="s">
-        <v>380</v>
+        <v>384</v>
       </c>
       <c r="D285" s="29"/>
       <c r="E285" s="29" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="F285" s="29"/>
       <c r="G285" s="40">
@@ -9667,7 +9667,7 @@
       <c r="A286" s="23"/>
       <c r="B286" s="13"/>
       <c r="C286" s="13" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D286" s="29"/>
       <c r="E286" s="28"/>
@@ -9695,10 +9695,10 @@
       <c r="A287" s="23"/>
       <c r="B287" s="13"/>
       <c r="C287" s="13" t="s">
-        <v>381</v>
+        <v>385</v>
       </c>
       <c r="D287" s="29" t="s">
-        <v>382</v>
+        <v>386</v>
       </c>
       <c r="E287" s="28"/>
       <c r="G287" s="40">
@@ -9722,7 +9722,7 @@
       <c r="A288" s="23"/>
       <c r="B288" s="14"/>
       <c r="C288" s="14" t="s">
-        <v>383</v>
+        <v>387</v>
       </c>
       <c r="D288" s="29"/>
       <c r="E288" s="28"/>
@@ -9746,10 +9746,10 @@
     <row r="289" spans="1:11" ht="18.75" customHeight="1">
       <c r="A289" s="23"/>
       <c r="B289" s="17" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c r="C289" s="17" t="s">
-        <v>384</v>
+        <v>388</v>
       </c>
       <c r="D289" s="29"/>
       <c r="E289" s="28"/>
@@ -9777,7 +9777,7 @@
       <c r="A290" s="23"/>
       <c r="B290" s="17"/>
       <c r="C290" s="17" t="s">
-        <v>385</v>
+        <v>389</v>
       </c>
       <c r="D290" s="29"/>
       <c r="E290" s="28"/>
@@ -9827,7 +9827,7 @@
       <c r="A292" s="23"/>
       <c r="B292" s="17"/>
       <c r="C292" s="17" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="D292" s="29"/>
       <c r="E292" s="28"/>
@@ -9852,7 +9852,7 @@
       <c r="A293" s="23"/>
       <c r="B293" s="17"/>
       <c r="C293" s="17" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D293" s="29"/>
       <c r="E293" s="28"/>
@@ -9877,7 +9877,7 @@
       <c r="A294" s="23"/>
       <c r="B294" s="17"/>
       <c r="C294" s="17" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D294" s="29"/>
       <c r="E294" s="28"/>
@@ -9902,7 +9902,7 @@
       <c r="A295" s="23"/>
       <c r="B295" s="17"/>
       <c r="C295" s="17" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D295" s="29"/>
       <c r="E295" s="28"/>
@@ -9927,7 +9927,7 @@
       <c r="A296" s="23"/>
       <c r="B296" s="17"/>
       <c r="C296" s="17" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="D296" s="29"/>
       <c r="E296" s="28"/>
@@ -9952,7 +9952,7 @@
       <c r="A297" s="23"/>
       <c r="B297" s="17"/>
       <c r="C297" s="17" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D297" s="29"/>
       <c r="E297" s="28"/>
@@ -9977,7 +9977,7 @@
       <c r="A298" s="23"/>
       <c r="B298" s="17"/>
       <c r="C298" s="17" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D298" s="29"/>
       <c r="E298" s="28"/>
@@ -10002,7 +10002,7 @@
       <c r="A299" s="23"/>
       <c r="B299" s="17"/>
       <c r="C299" s="17" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D299" s="29"/>
       <c r="E299" s="28"/>
@@ -10027,7 +10027,7 @@
       <c r="A300" s="23"/>
       <c r="B300" s="17"/>
       <c r="C300" s="17" t="s">
-        <v>386</v>
+        <v>390</v>
       </c>
       <c r="D300" s="29"/>
       <c r="E300" s="28"/>
@@ -10052,7 +10052,7 @@
       <c r="A301" s="23"/>
       <c r="B301" s="18"/>
       <c r="C301" s="18" t="s">
-        <v>387</v>
+        <v>391</v>
       </c>
       <c r="D301" s="29"/>
       <c r="E301" s="28"/>
@@ -10076,7 +10076,7 @@
     <row r="302" spans="1:11" ht="18.75" customHeight="1">
       <c r="A302" s="23"/>
       <c r="B302" s="17" t="s">
-        <v>345</v>
+        <v>349</v>
       </c>
       <c r="C302" s="17" t="s">
         <v>22</v>
@@ -10107,7 +10107,7 @@
       <c r="A303" s="23"/>
       <c r="B303" s="18"/>
       <c r="C303" s="18" t="s">
-        <v>388</v>
+        <v>392</v>
       </c>
       <c r="D303" s="29"/>
       <c r="E303" s="28"/>
@@ -10131,10 +10131,10 @@
     <row r="304" spans="1:11" ht="18.75" customHeight="1">
       <c r="A304" s="23"/>
       <c r="B304" s="17" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C304" s="17" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="D304" s="29"/>
       <c r="E304" s="28"/>
@@ -10162,7 +10162,7 @@
       <c r="A305" s="23"/>
       <c r="B305" s="17"/>
       <c r="C305" s="17" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="D305" s="29"/>
       <c r="E305" s="28"/>
@@ -10187,7 +10187,7 @@
       <c r="A306" s="23"/>
       <c r="B306" s="17"/>
       <c r="C306" s="17" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="D306" s="29"/>
       <c r="E306" s="28"/>
@@ -10212,7 +10212,7 @@
       <c r="A307" s="23"/>
       <c r="B307" s="17"/>
       <c r="C307" s="17" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
       <c r="D307" s="29"/>
       <c r="E307" s="28"/>
@@ -10237,7 +10237,7 @@
       <c r="A308" s="23"/>
       <c r="B308" s="17"/>
       <c r="C308" s="17" t="s">
-        <v>391</v>
+        <v>395</v>
       </c>
       <c r="D308" s="29"/>
       <c r="E308" s="28"/>
@@ -10262,7 +10262,7 @@
       <c r="A309" s="23"/>
       <c r="B309" s="17"/>
       <c r="C309" s="17" t="s">
-        <v>392</v>
+        <v>396</v>
       </c>
       <c r="D309" s="29"/>
       <c r="E309" s="28"/>
@@ -10287,10 +10287,10 @@
       <c r="A310" s="23"/>
       <c r="B310" s="17"/>
       <c r="C310" s="18" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="D310" s="29" t="s">
-        <v>394</v>
+        <v>398</v>
       </c>
       <c r="E310" s="28"/>
       <c r="G310" s="40">
@@ -10342,7 +10342,7 @@
       <c r="A312" s="23"/>
       <c r="B312" s="17"/>
       <c r="C312" s="17" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D312" s="29"/>
       <c r="E312" s="28"/>
@@ -10367,7 +10367,7 @@
       <c r="A313" s="23"/>
       <c r="B313" s="17"/>
       <c r="C313" s="17" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="D313" s="29"/>
       <c r="E313" s="28"/>
@@ -10392,7 +10392,7 @@
       <c r="A314" s="23"/>
       <c r="B314" s="17"/>
       <c r="C314" s="17" t="s">
-        <v>396</v>
+        <v>400</v>
       </c>
       <c r="D314" s="29"/>
       <c r="E314" s="28"/>
@@ -10416,10 +10416,10 @@
     <row r="315" spans="1:11" ht="18.75" customHeight="1">
       <c r="A315" s="23"/>
       <c r="B315" s="12" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C315" s="12" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D315" s="29"/>
       <c r="E315" s="28"/>
@@ -10447,10 +10447,10 @@
       <c r="A316" s="23"/>
       <c r="B316" s="13"/>
       <c r="C316" s="13" t="s">
-        <v>397</v>
+        <v>401</v>
       </c>
       <c r="D316" s="29" t="s">
-        <v>398</v>
+        <v>402</v>
       </c>
       <c r="E316" s="28"/>
       <c r="G316" s="40">
@@ -10499,7 +10499,7 @@
       <c r="A318" s="23"/>
       <c r="B318" s="13"/>
       <c r="C318" s="13" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D318" s="29"/>
       <c r="E318" s="28"/>
@@ -10524,7 +10524,7 @@
       <c r="A319" s="23"/>
       <c r="B319" s="13"/>
       <c r="C319" s="13" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D319" s="29"/>
       <c r="E319" s="28"/>
@@ -10549,7 +10549,7 @@
       <c r="A320" s="23"/>
       <c r="B320" s="14"/>
       <c r="C320" s="14" t="s">
-        <v>399</v>
+        <v>403</v>
       </c>
       <c r="D320" s="29"/>
       <c r="E320" s="28"/>
@@ -10573,10 +10573,10 @@
     <row r="321" spans="1:11" ht="18.75" customHeight="1">
       <c r="A321" s="23"/>
       <c r="B321" s="17" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
       <c r="C321" s="17" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
       <c r="D321" s="29"/>
       <c r="E321" s="28"/>
@@ -10604,7 +10604,7 @@
       <c r="A322" s="23"/>
       <c r="B322" s="17"/>
       <c r="C322" s="17" t="s">
-        <v>401</v>
+        <v>405</v>
       </c>
       <c r="D322" s="29"/>
       <c r="E322" s="28"/>
@@ -10629,7 +10629,7 @@
       <c r="A323" s="23"/>
       <c r="B323" s="18"/>
       <c r="C323" s="18" t="s">
-        <v>402</v>
+        <v>406</v>
       </c>
       <c r="D323" s="29"/>
       <c r="E323" s="28"/>
@@ -10653,13 +10653,13 @@
     <row r="324" spans="1:11" ht="18.75" customHeight="1">
       <c r="A324" s="23"/>
       <c r="B324" s="12" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C324" s="12" t="s">
-        <v>403</v>
+        <v>407</v>
       </c>
       <c r="D324" s="29" t="s">
-        <v>404</v>
+        <v>408</v>
       </c>
       <c r="E324" s="28"/>
       <c r="G324" s="40">
@@ -10686,10 +10686,10 @@
       <c r="A325" s="23"/>
       <c r="B325" s="13"/>
       <c r="C325" s="13" t="s">
-        <v>405</v>
+        <v>409</v>
       </c>
       <c r="D325" s="29" t="s">
-        <v>406</v>
+        <v>410</v>
       </c>
       <c r="E325" s="28"/>
       <c r="G325" s="40">
@@ -10713,7 +10713,7 @@
       <c r="A326" s="23"/>
       <c r="B326" s="14"/>
       <c r="C326" s="14" t="s">
-        <v>407</v>
+        <v>411</v>
       </c>
       <c r="D326" s="29"/>
       <c r="E326" s="28"/>
@@ -10737,10 +10737,10 @@
     <row r="327" spans="1:11" ht="18.75" customHeight="1">
       <c r="A327" s="23"/>
       <c r="B327" s="17" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C327" s="17" t="s">
-        <v>408</v>
+        <v>412</v>
       </c>
       <c r="D327" s="29"/>
       <c r="E327" s="28"/>
@@ -10768,10 +10768,10 @@
       <c r="A328" s="23"/>
       <c r="B328" s="17"/>
       <c r="C328" s="17" t="s">
-        <v>409</v>
+        <v>413</v>
       </c>
       <c r="D328" s="29" t="s">
-        <v>410</v>
+        <v>414</v>
       </c>
       <c r="E328" s="28"/>
       <c r="G328" s="40">
@@ -10795,7 +10795,7 @@
       <c r="A329" s="23"/>
       <c r="B329" s="18"/>
       <c r="C329" s="18" t="s">
-        <v>411</v>
+        <v>415</v>
       </c>
       <c r="D329" s="29"/>
       <c r="E329" s="28"/>
@@ -10819,10 +10819,10 @@
     <row r="330" spans="1:11" ht="18.75" customHeight="1">
       <c r="A330" s="23"/>
       <c r="B330" s="12" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C330" s="12" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D330" s="29"/>
       <c r="E330" s="28"/>
@@ -10850,7 +10850,7 @@
       <c r="A331" s="23"/>
       <c r="B331" s="14"/>
       <c r="C331" s="14" t="s">
-        <v>412</v>
+        <v>416</v>
       </c>
       <c r="D331" s="29"/>
       <c r="E331" s="28"/>
@@ -10874,10 +10874,10 @@
     <row r="332" spans="1:11" ht="18.75" customHeight="1" thickBot="1">
       <c r="A332" s="23"/>
       <c r="B332" s="18" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C332" s="18" t="s">
-        <v>413</v>
+        <v>417</v>
       </c>
       <c r="D332" s="29"/>
       <c r="E332" s="28"/>
@@ -10904,10 +10904,10 @@
     <row r="333" spans="1:11" ht="18.75" customHeight="1">
       <c r="A333" s="23"/>
       <c r="B333" s="17" t="s">
-        <v>421</v>
+        <v>425</v>
       </c>
       <c r="C333" s="17" t="s">
-        <v>414</v>
+        <v>418</v>
       </c>
       <c r="D333" s="29"/>
       <c r="E333" s="28"/>
@@ -10935,7 +10935,7 @@
       <c r="A334" s="23"/>
       <c r="B334" s="17"/>
       <c r="C334" s="17" t="s">
-        <v>415</v>
+        <v>419</v>
       </c>
       <c r="D334" s="29"/>
       <c r="E334" s="28"/>
@@ -10989,10 +10989,10 @@
     <row r="336" spans="1:11" ht="18.75" customHeight="1">
       <c r="A336" s="23"/>
       <c r="B336" s="12" t="s">
-        <v>418</v>
+        <v>422</v>
       </c>
       <c r="C336" s="12" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="D336" s="29"/>
       <c r="E336" s="28"/>
@@ -11020,7 +11020,7 @@
       <c r="A337" s="23"/>
       <c r="B337" s="13"/>
       <c r="C337" s="13" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="D337" s="29"/>
       <c r="E337" s="28"/>
@@ -11045,7 +11045,7 @@
       <c r="A338" s="23"/>
       <c r="B338" s="13"/>
       <c r="C338" s="13" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="D338" s="29"/>
       <c r="E338" s="28"/>
@@ -11070,7 +11070,7 @@
       <c r="A339" s="23"/>
       <c r="B339" s="13"/>
       <c r="C339" s="13" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="D339" s="29"/>
       <c r="E339" s="28"/>
@@ -11095,7 +11095,7 @@
       <c r="A340" s="23"/>
       <c r="B340" s="13"/>
       <c r="C340" s="13" t="s">
-        <v>416</v>
+        <v>420</v>
       </c>
       <c r="D340" s="29"/>
       <c r="E340" s="28"/>
@@ -11120,7 +11120,7 @@
       <c r="A341" s="23"/>
       <c r="B341" s="13"/>
       <c r="C341" s="13" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D341" s="29"/>
       <c r="E341" s="28"/>
@@ -11145,7 +11145,7 @@
       <c r="A342" s="23"/>
       <c r="B342" s="13"/>
       <c r="C342" s="13" t="s">
-        <v>417</v>
+        <v>421</v>
       </c>
       <c r="D342" s="29"/>
       <c r="E342" s="28"/>
@@ -11170,7 +11170,7 @@
       <c r="A343" s="23"/>
       <c r="B343" s="13"/>
       <c r="C343" s="13" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D343" s="29"/>
       <c r="E343" s="28"/>
@@ -11195,7 +11195,7 @@
       <c r="A344" s="23"/>
       <c r="B344" s="13"/>
       <c r="C344" s="13" t="s">
-        <v>425</v>
+        <v>428</v>
       </c>
       <c r="D344" s="29"/>
       <c r="E344" s="28"/>
@@ -11220,7 +11220,7 @@
       <c r="A345" s="23"/>
       <c r="B345" s="13"/>
       <c r="C345" s="13" t="s">
-        <v>426</v>
+        <v>429</v>
       </c>
       <c r="D345" s="29"/>
       <c r="E345" s="28"/>
@@ -11245,7 +11245,7 @@
       <c r="A346" s="23"/>
       <c r="B346" s="13"/>
       <c r="C346" s="13" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="D346" s="29"/>
       <c r="E346" s="28"/>
@@ -11270,7 +11270,7 @@
       <c r="A347" s="23"/>
       <c r="B347" s="13"/>
       <c r="C347" s="13" t="s">
-        <v>427</v>
+        <v>430</v>
       </c>
       <c r="D347" s="29"/>
       <c r="E347" s="28"/>
@@ -11295,7 +11295,7 @@
       <c r="A348" s="23"/>
       <c r="B348" s="13"/>
       <c r="C348" s="13" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D348" s="29"/>
       <c r="E348" s="28"/>
@@ -11320,7 +11320,7 @@
       <c r="A349" s="23"/>
       <c r="B349" s="13"/>
       <c r="C349" s="13" t="s">
-        <v>428</v>
+        <v>431</v>
       </c>
       <c r="D349" s="29"/>
       <c r="E349" s="28"/>
@@ -11345,7 +11345,7 @@
       <c r="A350" s="23"/>
       <c r="B350" s="13"/>
       <c r="C350" s="13" t="s">
-        <v>429</v>
+        <v>432</v>
       </c>
       <c r="D350" s="29"/>
       <c r="E350" s="28"/>
@@ -11370,7 +11370,7 @@
       <c r="A351" s="23"/>
       <c r="B351" s="13"/>
       <c r="C351" s="13" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D351" s="29"/>
       <c r="E351" s="28"/>
@@ -11395,7 +11395,7 @@
       <c r="A352" s="23"/>
       <c r="B352" s="13"/>
       <c r="C352" s="13" t="s">
-        <v>430</v>
+        <v>433</v>
       </c>
       <c r="D352" s="29"/>
       <c r="E352" s="28"/>
@@ -11419,10 +11419,10 @@
     <row r="353" spans="1:11" ht="18.75" customHeight="1">
       <c r="A353" s="23"/>
       <c r="B353" s="26" t="s">
-        <v>422</v>
+        <v>426</v>
       </c>
       <c r="C353" s="12" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
       <c r="D353" s="29"/>
       <c r="E353" s="28"/>
@@ -11450,7 +11450,7 @@
       <c r="A354" s="23"/>
       <c r="B354" s="13"/>
       <c r="C354" s="39" t="s">
-        <v>432</v>
+        <v>435</v>
       </c>
       <c r="D354" s="29"/>
       <c r="E354" s="28"/>
@@ -11475,7 +11475,7 @@
       <c r="A355" s="23"/>
       <c r="B355" s="13"/>
       <c r="C355" s="39" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
       <c r="D355" s="29"/>
       <c r="E355" s="28"/>
@@ -11500,7 +11500,7 @@
       <c r="A356" s="23"/>
       <c r="B356" s="13"/>
       <c r="C356" s="39" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="D356" s="29"/>
       <c r="E356" s="28"/>
@@ -11525,7 +11525,7 @@
       <c r="A357" s="23"/>
       <c r="B357" s="13"/>
       <c r="C357" s="39" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D357" s="29"/>
       <c r="E357" s="28"/>
@@ -11550,7 +11550,7 @@
       <c r="A358" s="23"/>
       <c r="B358" s="13"/>
       <c r="C358" s="14" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="D358" s="29"/>
       <c r="E358" s="28"/>
@@ -11574,10 +11574,10 @@
     <row r="359" spans="1:11" ht="18.75" customHeight="1" thickBot="1">
       <c r="A359" s="23"/>
       <c r="B359" s="19" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
       <c r="C359" s="19" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="D359" s="29"/>
       <c r="E359" s="28"/>
@@ -11604,10 +11604,10 @@
     <row r="360" spans="1:11" ht="18.75" customHeight="1" thickBot="1">
       <c r="A360" s="23"/>
       <c r="B360" s="15" t="s">
-        <v>424</v>
+        <v>454</v>
       </c>
       <c r="C360" s="15" t="s">
-        <v>436</v>
+        <v>439</v>
       </c>
       <c r="D360" s="29"/>
       <c r="E360" s="28"/>
@@ -11634,10 +11634,10 @@
     <row r="361" spans="1:11" ht="18.75" customHeight="1" thickBot="1">
       <c r="A361" s="18"/>
       <c r="B361" s="19" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="C361" s="19" t="s">
-        <v>437</v>
+        <v>440</v>
       </c>
       <c r="D361" s="29"/>
       <c r="E361" s="28"/>

</xml_diff>

<commit_message>
Changed default status of most diagnoses for testing.
</commit_message>
<xml_diff>
--- a/basis/Diagnosis_mapper_source.xlsx
+++ b/basis/Diagnosis_mapper_source.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\weberj3\Documents\git\dermodelphi\basis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\weberj3\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FE9F4E7-2177-4364-8F1E-DC9B6E08E515}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{61C41826-65D1-4E58-BB8F-DD8C579CF245}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="460">
   <si>
     <t>Benign</t>
   </si>
@@ -1122,12 +1122,6 @@
     <t>Exogenous, other (to be specified)</t>
   </si>
   <si>
-    <t>Benign, other (to be specified)</t>
-  </si>
-  <si>
-    <t>Benign - Other or not readily classifiable</t>
-  </si>
-  <si>
     <t>Adnexal epithelial proliferations - Apocrine or Eccrine</t>
   </si>
   <si>
@@ -1434,9 +1428,6 @@
     <t>Superficial (Ackerman nevus);Superficial and deep (Zitelli nevus);Deep (Mark nevus)</t>
   </si>
   <si>
-    <t>Malignant – Other (or not readily classifiable)</t>
-  </si>
-  <si>
     <t>Nevus, Congenital pattern (per histopathology)</t>
   </si>
   <si>
@@ -1461,10 +1452,25 @@
     <t>Collision - Only benign proliferations</t>
   </si>
   <si>
+    <t>Malignant – Other</t>
+  </si>
+  <si>
+    <t>Benign - Other</t>
+  </si>
+  <si>
+    <t>Benign, other (or not readily classifiable; to be specified)</t>
+  </si>
+  <si>
+    <t>Compound nevus;Dermal (intradermal) nevus</t>
+  </si>
+  <si>
     <t>Status</t>
   </si>
   <si>
     <t>visible</t>
+  </si>
+  <si>
+    <t>locked</t>
   </si>
 </sst>
 </file>
@@ -2118,7 +2124,7 @@
         <v>214</v>
       </c>
       <c r="L1" s="38" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="18.75" customHeight="1">
@@ -2152,7 +2158,7 @@
         <v>1010101</v>
       </c>
       <c r="L2" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="18.75" customHeight="1">
@@ -2180,7 +2186,7 @@
         <v>1010102</v>
       </c>
       <c r="L3" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
@@ -2208,7 +2214,7 @@
         <v>1010103</v>
       </c>
       <c r="L4" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="18.75" customHeight="1">
@@ -2219,7 +2225,7 @@
       </c>
       <c r="D5" s="29"/>
       <c r="E5" s="29" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="F5" s="29"/>
       <c r="G5" s="40">
@@ -2242,7 +2248,7 @@
         <v>1010201</v>
       </c>
       <c r="L5" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="18.75" customHeight="1">
@@ -2253,7 +2259,7 @@
       </c>
       <c r="D6" s="29"/>
       <c r="E6" s="29" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="F6" s="29"/>
       <c r="G6" s="40">
@@ -2273,7 +2279,7 @@
         <v>1010202</v>
       </c>
       <c r="L6" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
@@ -2284,7 +2290,7 @@
       </c>
       <c r="D7" s="29"/>
       <c r="E7" s="29" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="F7" s="29"/>
       <c r="G7" s="40">
@@ -2304,7 +2310,7 @@
         <v>1010203</v>
       </c>
       <c r="L7" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="18.75" customHeight="1">
@@ -2317,7 +2323,7 @@
         <v>264</v>
       </c>
       <c r="E8" s="29" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="F8" s="29"/>
       <c r="G8" s="40">
@@ -2340,7 +2346,7 @@
         <v>1010301</v>
       </c>
       <c r="L8" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="18.75" customHeight="1">
@@ -2353,7 +2359,7 @@
         <v>263</v>
       </c>
       <c r="E9" s="29" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="F9" s="29"/>
       <c r="G9" s="40">
@@ -2373,7 +2379,7 @@
         <v>1010302</v>
       </c>
       <c r="L9" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="18.75" customHeight="1">
@@ -2384,7 +2390,7 @@
       </c>
       <c r="D10" s="29"/>
       <c r="E10" s="29" t="s">
-        <v>450</v>
+        <v>456</v>
       </c>
       <c r="F10" s="29"/>
       <c r="G10" s="40">
@@ -2404,7 +2410,7 @@
         <v>1010303</v>
       </c>
       <c r="L10" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="18.75" customHeight="1">
@@ -2415,7 +2421,7 @@
       </c>
       <c r="D11" s="29"/>
       <c r="E11" s="29" t="s">
-        <v>450</v>
+        <v>456</v>
       </c>
       <c r="F11" s="29"/>
       <c r="G11" s="40">
@@ -2435,20 +2441,20 @@
         <v>1010304</v>
       </c>
       <c r="L11" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
       <c r="A12" s="31"/>
       <c r="B12" s="3"/>
       <c r="C12" s="4" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="D12" s="29" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="E12" s="29" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="F12" s="29"/>
       <c r="G12" s="40">
@@ -2468,7 +2474,7 @@
         <v>1010305</v>
       </c>
       <c r="L12" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="18.75" customHeight="1">
@@ -2479,10 +2485,10 @@
       </c>
       <c r="D13" s="29"/>
       <c r="E13" s="29" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="F13" s="29" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="G13" s="40">
         <f t="shared" si="0"/>
@@ -2504,21 +2510,21 @@
         <v>1010401</v>
       </c>
       <c r="L13" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
       <c r="A14" s="31"/>
       <c r="B14" s="3"/>
       <c r="C14" s="6" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="D14" s="29"/>
       <c r="E14" s="29" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="F14" s="29" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="G14" s="40">
         <f t="shared" si="0"/>
@@ -2537,7 +2543,7 @@
         <v>1010402</v>
       </c>
       <c r="L14" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="18.75" customHeight="1">
@@ -2568,7 +2574,7 @@
         <v>1010501</v>
       </c>
       <c r="L15" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
@@ -2596,7 +2602,7 @@
         <v>1010502</v>
       </c>
       <c r="L16" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="18.75" customHeight="1">
@@ -2627,7 +2633,7 @@
         <v>1010601</v>
       </c>
       <c r="L17" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="18.75" customHeight="1">
@@ -2657,7 +2663,7 @@
         <v>1010602</v>
       </c>
       <c r="L18" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="18.75" customHeight="1">
@@ -2687,7 +2693,7 @@
         <v>1010603</v>
       </c>
       <c r="L19" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="18.75" customHeight="1">
@@ -2715,7 +2721,7 @@
         <v>1010604</v>
       </c>
       <c r="L20" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
@@ -2745,7 +2751,7 @@
         <v>1010605</v>
       </c>
       <c r="L21" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="18.75" customHeight="1">
@@ -2776,7 +2782,7 @@
         <v>1010701</v>
       </c>
       <c r="L22" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
@@ -2804,7 +2810,7 @@
         <v>1010702</v>
       </c>
       <c r="L23" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="18.75" customHeight="1">
@@ -2815,7 +2821,7 @@
       </c>
       <c r="D24" s="29"/>
       <c r="E24" s="29" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="F24" s="29"/>
       <c r="G24" s="40">
@@ -2838,7 +2844,7 @@
         <v>1010801</v>
       </c>
       <c r="L24" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="18.75" customHeight="1">
@@ -2849,7 +2855,7 @@
       </c>
       <c r="D25" s="29"/>
       <c r="E25" s="29" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="F25" s="29"/>
       <c r="G25" s="40">
@@ -2869,7 +2875,7 @@
         <v>1010802</v>
       </c>
       <c r="L25" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="18.75" customHeight="1">
@@ -2880,7 +2886,7 @@
       </c>
       <c r="D26" s="29"/>
       <c r="E26" s="29" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="F26" s="29"/>
       <c r="G26" s="40">
@@ -2900,7 +2906,7 @@
         <v>1010803</v>
       </c>
       <c r="L26" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="18.75" customHeight="1">
@@ -2913,7 +2919,7 @@
         <v>234</v>
       </c>
       <c r="E27" s="29" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="F27" s="29"/>
       <c r="G27" s="40">
@@ -2933,7 +2939,7 @@
         <v>1010804</v>
       </c>
       <c r="L27" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="18.75" customHeight="1">
@@ -2944,7 +2950,7 @@
       </c>
       <c r="D28" s="29"/>
       <c r="E28" s="29" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="F28" s="29"/>
       <c r="G28" s="40">
@@ -2964,7 +2970,7 @@
         <v>1010805</v>
       </c>
       <c r="L28" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
@@ -2977,7 +2983,7 @@
         <v>228</v>
       </c>
       <c r="E29" s="29" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="F29" s="29"/>
       <c r="G29" s="40">
@@ -2997,7 +3003,7 @@
         <v>1010806</v>
       </c>
       <c r="L29" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
@@ -3030,7 +3036,7 @@
         <v>1010901</v>
       </c>
       <c r="L30" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="18.75" customHeight="1">
@@ -3061,7 +3067,7 @@
         <v>1011001</v>
       </c>
       <c r="L31" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="18.75" customHeight="1">
@@ -3089,7 +3095,7 @@
         <v>1011002</v>
       </c>
       <c r="L32" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="33" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
@@ -3117,7 +3123,7 @@
         <v>1011003</v>
       </c>
       <c r="L33" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
@@ -3148,7 +3154,7 @@
         <v>1011101</v>
       </c>
       <c r="L34" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="35" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
@@ -3179,7 +3185,7 @@
         <v>1011201</v>
       </c>
       <c r="L35" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="18.75" customHeight="1">
@@ -3214,7 +3220,7 @@
         <v>1020101</v>
       </c>
       <c r="L36" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="18.75" customHeight="1">
@@ -3244,7 +3250,7 @@
         <v>1020102</v>
       </c>
       <c r="L37" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="38" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
@@ -3272,7 +3278,7 @@
         <v>1020103</v>
       </c>
       <c r="L38" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="39" spans="1:12" ht="18.75" customHeight="1">
@@ -3305,7 +3311,7 @@
         <v>1030101</v>
       </c>
       <c r="L39" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="40" spans="1:12" ht="18.75" customHeight="1">
@@ -3333,7 +3339,7 @@
         <v>1030102</v>
       </c>
       <c r="L40" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
@@ -3363,7 +3369,7 @@
         <v>1030103</v>
       </c>
       <c r="L41" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="18.75" customHeight="1">
@@ -3396,7 +3402,7 @@
         <v>1030201</v>
       </c>
       <c r="L42" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="18.75" customHeight="1">
@@ -3424,7 +3430,7 @@
         <v>1030202</v>
       </c>
       <c r="L43" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="44" spans="1:12" ht="18.75" customHeight="1">
@@ -3452,7 +3458,7 @@
         <v>1030203</v>
       </c>
       <c r="L44" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="45" spans="1:12" ht="18.75" customHeight="1">
@@ -3480,7 +3486,7 @@
         <v>1030204</v>
       </c>
       <c r="L45" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="46" spans="1:12" ht="18.75" customHeight="1">
@@ -3508,7 +3514,7 @@
         <v>1030205</v>
       </c>
       <c r="L46" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="47" spans="1:12" ht="18.75" customHeight="1">
@@ -3536,7 +3542,7 @@
         <v>1030206</v>
       </c>
       <c r="L47" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="48" spans="1:12" ht="18.75" customHeight="1">
@@ -3564,7 +3570,7 @@
         <v>1030207</v>
       </c>
       <c r="L48" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="49" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
@@ -3592,13 +3598,13 @@
         <v>1030208</v>
       </c>
       <c r="L49" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="50" spans="1:12" ht="18.75" customHeight="1">
       <c r="A50" s="31"/>
       <c r="B50" s="5" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>76</v>
@@ -3625,7 +3631,7 @@
         <v>1040101</v>
       </c>
       <c r="L50" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="51" spans="1:12" ht="18.75" customHeight="1">
@@ -3655,7 +3661,7 @@
         <v>1040102</v>
       </c>
       <c r="L51" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="52" spans="1:12" ht="18.75" customHeight="1">
@@ -3683,7 +3689,7 @@
         <v>1040103</v>
       </c>
       <c r="L52" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="53" spans="1:12" ht="18.75" customHeight="1">
@@ -3711,7 +3717,7 @@
         <v>1040104</v>
       </c>
       <c r="L53" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="54" spans="1:12" ht="18.75" customHeight="1">
@@ -3739,7 +3745,7 @@
         <v>1040105</v>
       </c>
       <c r="L54" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="55" spans="1:12" ht="18.75" customHeight="1">
@@ -3767,7 +3773,7 @@
         <v>1040106</v>
       </c>
       <c r="L55" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="56" spans="1:12" ht="18.75" customHeight="1">
@@ -3795,7 +3801,7 @@
         <v>1040107</v>
       </c>
       <c r="L56" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="57" spans="1:12" ht="18.75" customHeight="1">
@@ -3823,7 +3829,7 @@
         <v>1040108</v>
       </c>
       <c r="L57" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="58" spans="1:12" ht="18.75" customHeight="1">
@@ -3851,7 +3857,7 @@
         <v>1040109</v>
       </c>
       <c r="L58" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="59" spans="1:12" ht="18.75" customHeight="1">
@@ -3879,7 +3885,7 @@
         <v>1040110</v>
       </c>
       <c r="L59" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="60" spans="1:12" ht="18.75" customHeight="1">
@@ -3907,7 +3913,7 @@
         <v>1040111</v>
       </c>
       <c r="L60" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="61" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
@@ -3935,13 +3941,13 @@
         <v>1040112</v>
       </c>
       <c r="L61" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="62" spans="1:12" ht="18.75" customHeight="1">
       <c r="A62" s="31"/>
       <c r="B62" s="2" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>6</v>
@@ -3968,7 +3974,7 @@
         <v>1050101</v>
       </c>
       <c r="L62" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="63" spans="1:12" ht="18.75" customHeight="1">
@@ -3996,7 +4002,7 @@
         <v>1050102</v>
       </c>
       <c r="L63" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="64" spans="1:12" ht="18.75" customHeight="1">
@@ -4024,7 +4030,7 @@
         <v>1050103</v>
       </c>
       <c r="L64" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="65" spans="1:12" ht="18.75" customHeight="1">
@@ -4052,7 +4058,7 @@
         <v>1050104</v>
       </c>
       <c r="L65" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="66" spans="1:12" ht="18.75" customHeight="1">
@@ -4082,7 +4088,7 @@
         <v>1050105</v>
       </c>
       <c r="L66" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="67" spans="1:12" ht="18.75" customHeight="1">
@@ -4110,7 +4116,7 @@
         <v>1050106</v>
       </c>
       <c r="L67" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="68" spans="1:12" ht="18.75" customHeight="1">
@@ -4138,14 +4144,14 @@
         <v>1050107</v>
       </c>
       <c r="L68" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="69" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
       <c r="A69" s="31"/>
       <c r="B69" s="4"/>
       <c r="C69" s="4" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="D69" s="29"/>
       <c r="E69" s="28"/>
@@ -4166,13 +4172,13 @@
         <v>1050108</v>
       </c>
       <c r="L69" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="70" spans="1:12" ht="18.75" customHeight="1">
       <c r="A70" s="31"/>
       <c r="B70" s="5" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C70" s="5" t="s">
         <v>8</v>
@@ -4199,7 +4205,7 @@
         <v>1060101</v>
       </c>
       <c r="L70" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="71" spans="1:12" ht="18.75" customHeight="1">
@@ -4227,7 +4233,7 @@
         <v>1060102</v>
       </c>
       <c r="L71" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="72" spans="1:12" ht="18.75" customHeight="1">
@@ -4255,14 +4261,14 @@
         <v>1060103</v>
       </c>
       <c r="L72" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="73" spans="1:12" ht="18.75" customHeight="1">
       <c r="A73" s="31"/>
       <c r="B73" s="7"/>
       <c r="C73" s="7" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="D73" s="29"/>
       <c r="E73" s="28"/>
@@ -4283,7 +4289,7 @@
         <v>1060104</v>
       </c>
       <c r="L73" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="74" spans="1:12" ht="18.75" customHeight="1">
@@ -4311,7 +4317,7 @@
         <v>1060105</v>
       </c>
       <c r="L74" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="75" spans="1:12" ht="18.75" customHeight="1">
@@ -4339,7 +4345,7 @@
         <v>1060106</v>
       </c>
       <c r="L75" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="76" spans="1:12" ht="18.75" customHeight="1">
@@ -4367,7 +4373,7 @@
         <v>1060107</v>
       </c>
       <c r="L76" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="77" spans="1:12" ht="18.75" customHeight="1">
@@ -4395,7 +4401,7 @@
         <v>1060108</v>
       </c>
       <c r="L77" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="78" spans="1:12" ht="18.75" customHeight="1">
@@ -4425,7 +4431,7 @@
         <v>1060109</v>
       </c>
       <c r="L78" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="79" spans="1:12" ht="18.75" customHeight="1">
@@ -4455,7 +4461,7 @@
         <v>1060110</v>
       </c>
       <c r="L79" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="80" spans="1:12" ht="18.75" customHeight="1">
@@ -4483,7 +4489,7 @@
         <v>1060111</v>
       </c>
       <c r="L80" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="81" spans="1:12" ht="18.75" customHeight="1">
@@ -4511,7 +4517,7 @@
         <v>1060112</v>
       </c>
       <c r="L81" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="82" spans="1:12" ht="18.75" customHeight="1">
@@ -4539,7 +4545,7 @@
         <v>1060113</v>
       </c>
       <c r="L82" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="83" spans="1:12" ht="18.75" customHeight="1">
@@ -4567,7 +4573,7 @@
         <v>1060114</v>
       </c>
       <c r="L83" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="84" spans="1:12" ht="18.75" customHeight="1">
@@ -4595,7 +4601,7 @@
         <v>1060115</v>
       </c>
       <c r="L84" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="85" spans="1:12" ht="18.75" customHeight="1">
@@ -4623,7 +4629,7 @@
         <v>1060116</v>
       </c>
       <c r="L85" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="86" spans="1:12" ht="18.75" customHeight="1">
@@ -4651,7 +4657,7 @@
         <v>1060117</v>
       </c>
       <c r="L86" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="87" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
@@ -4679,7 +4685,7 @@
         <v>1060118</v>
       </c>
       <c r="L87" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="88" spans="1:12" ht="18.75" customHeight="1">
@@ -4712,7 +4718,7 @@
         <v>1070101</v>
       </c>
       <c r="L88" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="89" spans="1:12" ht="18.75" customHeight="1">
@@ -4740,7 +4746,7 @@
         <v>1070102</v>
       </c>
       <c r="L89" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="90" spans="1:12" ht="18.75" customHeight="1">
@@ -4768,7 +4774,7 @@
         <v>1070103</v>
       </c>
       <c r="L90" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="91" spans="1:12" ht="18.75" customHeight="1">
@@ -4796,7 +4802,7 @@
         <v>1070104</v>
       </c>
       <c r="L91" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="92" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
@@ -4824,7 +4830,7 @@
         <v>1070105</v>
       </c>
       <c r="L92" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="93" spans="1:12" ht="18.75" customHeight="1">
@@ -4857,7 +4863,7 @@
         <v>1080101</v>
       </c>
       <c r="L93" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="94" spans="1:12" ht="18.75" customHeight="1">
@@ -4887,7 +4893,7 @@
         <v>1080102</v>
       </c>
       <c r="L94" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="95" spans="1:12" ht="18.75" customHeight="1">
@@ -4915,7 +4921,7 @@
         <v>1080103</v>
       </c>
       <c r="L95" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="96" spans="1:12" ht="18.75" customHeight="1">
@@ -4943,7 +4949,7 @@
         <v>1080104</v>
       </c>
       <c r="L96" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="97" spans="1:12" ht="18.75" customHeight="1">
@@ -4971,7 +4977,7 @@
         <v>1080105</v>
       </c>
       <c r="L97" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="98" spans="1:12" ht="18.75" customHeight="1">
@@ -4999,7 +5005,7 @@
         <v>1080106</v>
       </c>
       <c r="L98" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="99" spans="1:12" ht="18.75" customHeight="1">
@@ -5027,7 +5033,7 @@
         <v>1080107</v>
       </c>
       <c r="L99" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="100" spans="1:12" ht="18.75" customHeight="1">
@@ -5055,7 +5061,7 @@
         <v>1080108</v>
       </c>
       <c r="L100" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="101" spans="1:12" ht="18.75" customHeight="1">
@@ -5083,7 +5089,7 @@
         <v>1080109</v>
       </c>
       <c r="L101" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="102" spans="1:12" ht="18.75" customHeight="1">
@@ -5111,7 +5117,7 @@
         <v>1080110</v>
       </c>
       <c r="L102" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="103" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
@@ -5139,7 +5145,7 @@
         <v>1080111</v>
       </c>
       <c r="L103" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="104" spans="1:12" ht="18.75" customHeight="1">
@@ -5170,7 +5176,7 @@
         <v>1080201</v>
       </c>
       <c r="L104" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="105" spans="1:12" ht="18.75" customHeight="1">
@@ -5198,7 +5204,7 @@
         <v>1080202</v>
       </c>
       <c r="L105" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="106" spans="1:12" ht="18.75" customHeight="1">
@@ -5226,7 +5232,7 @@
         <v>1080203</v>
       </c>
       <c r="L106" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="107" spans="1:12" ht="18.75" customHeight="1">
@@ -5254,7 +5260,7 @@
         <v>1080204</v>
       </c>
       <c r="L107" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="108" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
@@ -5282,7 +5288,7 @@
         <v>1080205</v>
       </c>
       <c r="L108" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="109" spans="1:12" ht="18.75" customHeight="1">
@@ -5313,7 +5319,7 @@
         <v>1080301</v>
       </c>
       <c r="L109" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="110" spans="1:12" ht="18.75" customHeight="1">
@@ -5343,7 +5349,7 @@
         <v>1080302</v>
       </c>
       <c r="L110" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="111" spans="1:12" ht="18.75" customHeight="1">
@@ -5371,7 +5377,7 @@
         <v>1080303</v>
       </c>
       <c r="L111" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="112" spans="1:12" ht="18.75" customHeight="1">
@@ -5399,7 +5405,7 @@
         <v>1080304</v>
       </c>
       <c r="L112" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="113" spans="1:12" ht="18.75" customHeight="1">
@@ -5427,7 +5433,7 @@
         <v>1080305</v>
       </c>
       <c r="L113" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="114" spans="1:12" ht="18.75" customHeight="1">
@@ -5455,7 +5461,7 @@
         <v>1080306</v>
       </c>
       <c r="L114" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="115" spans="1:12" ht="18.75" customHeight="1">
@@ -5485,7 +5491,7 @@
         <v>1080307</v>
       </c>
       <c r="L115" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="116" spans="1:12" ht="18.75" customHeight="1">
@@ -5513,7 +5519,7 @@
         <v>1080308</v>
       </c>
       <c r="L116" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="117" spans="1:12" ht="18.75" customHeight="1">
@@ -5541,7 +5547,7 @@
         <v>1080309</v>
       </c>
       <c r="L117" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="118" spans="1:12" ht="18.75" customHeight="1">
@@ -5569,14 +5575,14 @@
         <v>1080310</v>
       </c>
       <c r="L118" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="119" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
       <c r="A119" s="31"/>
       <c r="B119" s="3"/>
       <c r="C119" s="3" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="D119" s="29"/>
       <c r="E119" s="28"/>
@@ -5597,7 +5603,7 @@
         <v>1080311</v>
       </c>
       <c r="L119" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="120" spans="1:12" ht="18.75" customHeight="1">
@@ -5609,7 +5615,7 @@
         <v>271</v>
       </c>
       <c r="D120" s="29" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="E120" s="28"/>
       <c r="G120" s="40">
@@ -5632,7 +5638,7 @@
         <v>1090101</v>
       </c>
       <c r="L120" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="121" spans="1:12" ht="18.75" customHeight="1">
@@ -5660,7 +5666,7 @@
         <v>1090102</v>
       </c>
       <c r="L121" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="122" spans="1:12" ht="18.75" customHeight="1">
@@ -5688,7 +5694,7 @@
         <v>1090103</v>
       </c>
       <c r="L122" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="123" spans="1:12" ht="18.75" customHeight="1">
@@ -5716,7 +5722,7 @@
         <v>1090104</v>
       </c>
       <c r="L123" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="124" spans="1:12" ht="18.75" customHeight="1">
@@ -5744,7 +5750,7 @@
         <v>1090105</v>
       </c>
       <c r="L124" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="125" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
@@ -5772,7 +5778,7 @@
         <v>1090106</v>
       </c>
       <c r="L125" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="126" spans="1:12" ht="18.75" customHeight="1">
@@ -5803,7 +5809,7 @@
         <v>1090201</v>
       </c>
       <c r="L126" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="127" spans="1:12" ht="18.75" customHeight="1">
@@ -5831,7 +5837,7 @@
         <v>1090202</v>
       </c>
       <c r="L127" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="128" spans="1:12" ht="18.75" customHeight="1">
@@ -5859,7 +5865,7 @@
         <v>1090203</v>
       </c>
       <c r="L128" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="129" spans="1:12" ht="18.75" customHeight="1">
@@ -5887,7 +5893,7 @@
         <v>1090204</v>
       </c>
       <c r="L129" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="130" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
@@ -5915,7 +5921,7 @@
         <v>1090205</v>
       </c>
       <c r="L130" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="131" spans="1:12" ht="18.75" customHeight="1">
@@ -5948,7 +5954,7 @@
         <v>1090301</v>
       </c>
       <c r="L131" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="132" spans="1:12" ht="18.75" customHeight="1">
@@ -5978,7 +5984,7 @@
         <v>1090302</v>
       </c>
       <c r="L132" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="133" spans="1:12" ht="18.75" customHeight="1">
@@ -6008,7 +6014,7 @@
         <v>1090303</v>
       </c>
       <c r="L133" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="134" spans="1:12" ht="18.75" customHeight="1">
@@ -6038,7 +6044,7 @@
         <v>1090304</v>
       </c>
       <c r="L134" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="135" spans="1:12" ht="18.75" customHeight="1">
@@ -6066,7 +6072,7 @@
         <v>1090305</v>
       </c>
       <c r="L135" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="136" spans="1:12" ht="18.75" customHeight="1">
@@ -6094,7 +6100,7 @@
         <v>1090306</v>
       </c>
       <c r="L136" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="137" spans="1:12" ht="18.75" customHeight="1">
@@ -6122,7 +6128,7 @@
         <v>1090307</v>
       </c>
       <c r="L137" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="138" spans="1:12" ht="18.75" customHeight="1">
@@ -6150,7 +6156,7 @@
         <v>1090308</v>
       </c>
       <c r="L138" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="139" spans="1:12" ht="18.75" customHeight="1">
@@ -6178,7 +6184,7 @@
         <v>1090309</v>
       </c>
       <c r="L139" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="140" spans="1:12" ht="18.75" customHeight="1">
@@ -6206,7 +6212,7 @@
         <v>1090310</v>
       </c>
       <c r="L140" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="141" spans="1:12" ht="18.75" customHeight="1">
@@ -6234,7 +6240,7 @@
         <v>1090311</v>
       </c>
       <c r="L141" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="142" spans="1:12" ht="18.75" customHeight="1">
@@ -6262,7 +6268,7 @@
         <v>1090312</v>
       </c>
       <c r="L142" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="143" spans="1:12" ht="18.75" customHeight="1">
@@ -6290,7 +6296,7 @@
         <v>1090313</v>
       </c>
       <c r="L143" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="144" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
@@ -6318,13 +6324,13 @@
         <v>1090314</v>
       </c>
       <c r="L144" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="145" spans="1:12" ht="18.75" customHeight="1">
       <c r="A145" s="31"/>
       <c r="B145" s="2" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="C145" s="2" t="s">
         <v>292</v>
@@ -6353,7 +6359,7 @@
         <v>1100101</v>
       </c>
       <c r="L145" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="146" spans="1:12" ht="18.75" customHeight="1">
@@ -6381,7 +6387,7 @@
         <v>1100102</v>
       </c>
       <c r="L146" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="147" spans="1:12" ht="18.75" customHeight="1">
@@ -6409,7 +6415,7 @@
         <v>1100103</v>
       </c>
       <c r="L147" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="148" spans="1:12" ht="18.75" customHeight="1">
@@ -6437,7 +6443,7 @@
         <v>1100104</v>
       </c>
       <c r="L148" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="149" spans="1:12" ht="18.75" customHeight="1">
@@ -6467,7 +6473,7 @@
         <v>1100105</v>
       </c>
       <c r="L149" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="150" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
@@ -6495,7 +6501,7 @@
         <v>1100106</v>
       </c>
       <c r="L150" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="151" spans="1:12" ht="18.75" customHeight="1">
@@ -6528,7 +6534,7 @@
         <v>1110101</v>
       </c>
       <c r="L151" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="152" spans="1:12" ht="18.75" customHeight="1">
@@ -6556,7 +6562,7 @@
         <v>1110102</v>
       </c>
       <c r="L152" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="153" spans="1:12" ht="18.75" customHeight="1">
@@ -6584,7 +6590,7 @@
         <v>1110103</v>
       </c>
       <c r="L153" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="154" spans="1:12" ht="18.75" customHeight="1">
@@ -6612,14 +6618,14 @@
         <v>1110104</v>
       </c>
       <c r="L154" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="155" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
       <c r="A155" s="31"/>
       <c r="B155" s="4"/>
       <c r="C155" s="4" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="D155" s="29"/>
       <c r="E155" s="28"/>
@@ -6640,7 +6646,7 @@
         <v>1110105</v>
       </c>
       <c r="L155" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="156" spans="1:12" ht="18.75" customHeight="1">
@@ -6673,7 +6679,7 @@
         <v>1120101</v>
       </c>
       <c r="L156" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="157" spans="1:12" ht="18.75" customHeight="1">
@@ -6701,7 +6707,7 @@
         <v>1120102</v>
       </c>
       <c r="L157" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="158" spans="1:12" ht="18.75" customHeight="1">
@@ -6729,7 +6735,7 @@
         <v>1120103</v>
       </c>
       <c r="L158" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="159" spans="1:12" ht="18.75" customHeight="1">
@@ -6757,7 +6763,7 @@
         <v>1120104</v>
       </c>
       <c r="L159" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="160" spans="1:12" ht="18.75" customHeight="1">
@@ -6785,7 +6791,7 @@
         <v>1120105</v>
       </c>
       <c r="L160" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="161" spans="1:12" ht="18.75" customHeight="1">
@@ -6813,7 +6819,7 @@
         <v>1120106</v>
       </c>
       <c r="L161" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="162" spans="1:12" ht="18.75" customHeight="1">
@@ -6841,7 +6847,7 @@
         <v>1120107</v>
       </c>
       <c r="L162" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="163" spans="1:12" ht="18.75" customHeight="1">
@@ -6869,7 +6875,7 @@
         <v>1120108</v>
       </c>
       <c r="L163" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="164" spans="1:12" ht="18.75" customHeight="1">
@@ -6897,7 +6903,7 @@
         <v>1120109</v>
       </c>
       <c r="L164" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="165" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
@@ -6925,7 +6931,7 @@
         <v>1120110</v>
       </c>
       <c r="L165" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="166" spans="1:12" ht="18.75" customHeight="1">
@@ -6958,7 +6964,7 @@
         <v>1130101</v>
       </c>
       <c r="L166" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="167" spans="1:12" ht="18.75" customHeight="1">
@@ -6986,7 +6992,7 @@
         <v>1130102</v>
       </c>
       <c r="L167" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="168" spans="1:12" ht="18.75" customHeight="1">
@@ -7016,7 +7022,7 @@
         <v>1130103</v>
       </c>
       <c r="L168" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="169" spans="1:12" ht="18.75" customHeight="1">
@@ -7044,7 +7050,7 @@
         <v>1130104</v>
       </c>
       <c r="L169" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="170" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
@@ -7072,7 +7078,7 @@
         <v>1130105</v>
       </c>
       <c r="L170" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="171" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
@@ -7105,7 +7111,7 @@
         <v>1140101</v>
       </c>
       <c r="L171" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="172" spans="1:12" ht="18.75" customHeight="1">
@@ -7138,7 +7144,7 @@
         <v>1150101</v>
       </c>
       <c r="L172" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="173" spans="1:12" ht="18.75" customHeight="1">
@@ -7166,7 +7172,7 @@
         <v>1150102</v>
       </c>
       <c r="L173" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="174" spans="1:12" ht="18.75" customHeight="1">
@@ -7196,14 +7202,14 @@
         <v>1150103</v>
       </c>
       <c r="L174" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="175" spans="1:12" ht="18.75" customHeight="1">
       <c r="A175" s="31"/>
       <c r="B175" s="3"/>
       <c r="C175" s="3" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="D175" s="29"/>
       <c r="E175" s="28"/>
@@ -7224,7 +7230,7 @@
         <v>1150104</v>
       </c>
       <c r="L175" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="176" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
@@ -7252,7 +7258,7 @@
         <v>1150105</v>
       </c>
       <c r="L176" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="177" spans="1:12" ht="18.75" customHeight="1">
@@ -7285,7 +7291,7 @@
         <v>1160101</v>
       </c>
       <c r="L177" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="178" spans="1:12" ht="18.75" customHeight="1">
@@ -7313,7 +7319,7 @@
         <v>1160102</v>
       </c>
       <c r="L178" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="179" spans="1:12" ht="18.75" customHeight="1">
@@ -7341,7 +7347,7 @@
         <v>1160103</v>
       </c>
       <c r="L179" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="180" spans="1:12" ht="18.75" customHeight="1">
@@ -7369,7 +7375,7 @@
         <v>1160104</v>
       </c>
       <c r="L180" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="181" spans="1:12" ht="18.75" customHeight="1">
@@ -7397,7 +7403,7 @@
         <v>1160105</v>
       </c>
       <c r="L181" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="182" spans="1:12" ht="18.75" customHeight="1">
@@ -7425,7 +7431,7 @@
         <v>1160106</v>
       </c>
       <c r="L182" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="183" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
@@ -7453,7 +7459,7 @@
         <v>1160107</v>
       </c>
       <c r="L183" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="184" spans="1:12" ht="18.75" customHeight="1">
@@ -7486,7 +7492,7 @@
         <v>1170101</v>
       </c>
       <c r="L184" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="185" spans="1:12" ht="18.75" customHeight="1">
@@ -7514,7 +7520,7 @@
         <v>1170102</v>
       </c>
       <c r="L185" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="186" spans="1:12" ht="18.75" customHeight="1">
@@ -7542,7 +7548,7 @@
         <v>1170103</v>
       </c>
       <c r="L186" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="187" spans="1:12" ht="18.75" customHeight="1">
@@ -7572,7 +7578,7 @@
         <v>1170104</v>
       </c>
       <c r="L187" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="188" spans="1:12" ht="18.75" customHeight="1">
@@ -7600,7 +7606,7 @@
         <v>1170105</v>
       </c>
       <c r="L188" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="189" spans="1:12" ht="18.75" customHeight="1">
@@ -7630,7 +7636,7 @@
         <v>1170106</v>
       </c>
       <c r="L189" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="190" spans="1:12" ht="18.75" customHeight="1">
@@ -7658,7 +7664,7 @@
         <v>1170107</v>
       </c>
       <c r="L190" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="191" spans="1:12" ht="18.75" customHeight="1">
@@ -7688,7 +7694,7 @@
         <v>1170108</v>
       </c>
       <c r="L191" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="192" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
@@ -7716,7 +7722,7 @@
         <v>1170109</v>
       </c>
       <c r="L192" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="193" spans="1:12" ht="18.75" customHeight="1">
@@ -7749,7 +7755,7 @@
         <v>1180101</v>
       </c>
       <c r="L193" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="194" spans="1:12" ht="18.75" customHeight="1">
@@ -7777,7 +7783,7 @@
         <v>1180102</v>
       </c>
       <c r="L194" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="195" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
@@ -7805,7 +7811,7 @@
         <v>1180103</v>
       </c>
       <c r="L195" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="196" spans="1:12" ht="18.75" customHeight="1">
@@ -7836,7 +7842,7 @@
         <v>1180201</v>
       </c>
       <c r="L196" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="197" spans="1:12" ht="18.75" customHeight="1">
@@ -7864,7 +7870,7 @@
         <v>1180202</v>
       </c>
       <c r="L197" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="198" spans="1:12" ht="18.75" customHeight="1">
@@ -7892,7 +7898,7 @@
         <v>1180203</v>
       </c>
       <c r="L198" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="199" spans="1:12" ht="18.75" customHeight="1">
@@ -7920,7 +7926,7 @@
         <v>1180204</v>
       </c>
       <c r="L199" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="200" spans="1:12" ht="18.75" customHeight="1">
@@ -7948,7 +7954,7 @@
         <v>1180205</v>
       </c>
       <c r="L200" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="201" spans="1:12" ht="18.75" customHeight="1">
@@ -7976,7 +7982,7 @@
         <v>1180206</v>
       </c>
       <c r="L201" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="202" spans="1:12" ht="18.75" customHeight="1">
@@ -8004,7 +8010,7 @@
         <v>1180207</v>
       </c>
       <c r="L202" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="203" spans="1:12" ht="18.75" customHeight="1">
@@ -8034,7 +8040,7 @@
         <v>1180208</v>
       </c>
       <c r="L203" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="204" spans="1:12" ht="18.75" customHeight="1">
@@ -8064,7 +8070,7 @@
         <v>1180209</v>
       </c>
       <c r="L204" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="205" spans="1:12" ht="18.75" customHeight="1">
@@ -8094,7 +8100,7 @@
         <v>1180210</v>
       </c>
       <c r="L205" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="206" spans="1:12" ht="18.75" customHeight="1">
@@ -8122,7 +8128,7 @@
         <v>1180211</v>
       </c>
       <c r="L206" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="207" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
@@ -8150,7 +8156,7 @@
         <v>1180212</v>
       </c>
       <c r="L207" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="208" spans="1:12" ht="18.75" customHeight="1">
@@ -8183,7 +8189,7 @@
         <v>1190101</v>
       </c>
       <c r="L208" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="209" spans="1:12" ht="18.75" customHeight="1">
@@ -8211,7 +8217,7 @@
         <v>1190102</v>
       </c>
       <c r="L209" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="210" spans="1:12" ht="18.75" customHeight="1">
@@ -8239,7 +8245,7 @@
         <v>1190103</v>
       </c>
       <c r="L210" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="211" spans="1:12" ht="18.75" customHeight="1">
@@ -8269,7 +8275,7 @@
         <v>1190104</v>
       </c>
       <c r="L211" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="212" spans="1:12" ht="18.75" customHeight="1">
@@ -8299,7 +8305,7 @@
         <v>1190105</v>
       </c>
       <c r="L212" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="213" spans="1:12" ht="18.75" customHeight="1">
@@ -8329,7 +8335,7 @@
         <v>1190106</v>
       </c>
       <c r="L213" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="214" spans="1:12" ht="18.75" customHeight="1">
@@ -8357,7 +8363,7 @@
         <v>1190107</v>
       </c>
       <c r="L214" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="215" spans="1:12" ht="18.75" customHeight="1">
@@ -8385,7 +8391,7 @@
         <v>1190108</v>
       </c>
       <c r="L215" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="216" spans="1:12" ht="18.75" customHeight="1">
@@ -8413,7 +8419,7 @@
         <v>1190109</v>
       </c>
       <c r="L216" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="217" spans="1:12" ht="18.75" customHeight="1">
@@ -8441,7 +8447,7 @@
         <v>1190110</v>
       </c>
       <c r="L217" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="218" spans="1:12" ht="18.75" customHeight="1">
@@ -8469,7 +8475,7 @@
         <v>1190111</v>
       </c>
       <c r="L218" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="219" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
@@ -8497,7 +8503,7 @@
         <v>1190112</v>
       </c>
       <c r="L219" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="220" spans="1:12" ht="18.75" customHeight="1">
@@ -8530,7 +8536,7 @@
         <v>1200101</v>
       </c>
       <c r="L220" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="221" spans="1:12" ht="18.75" customHeight="1">
@@ -8558,7 +8564,7 @@
         <v>1200102</v>
       </c>
       <c r="L221" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="222" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
@@ -8586,16 +8592,16 @@
         <v>1200103</v>
       </c>
       <c r="L222" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="223" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
       <c r="A223" s="31"/>
       <c r="B223" s="5" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="C223" s="10" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="D223" s="29"/>
       <c r="E223" s="28"/>
@@ -8619,16 +8625,16 @@
         <v>1210101</v>
       </c>
       <c r="L223" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="224" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
       <c r="A224" s="31"/>
       <c r="B224" s="11" t="s">
-        <v>344</v>
+        <v>454</v>
       </c>
       <c r="C224" s="11" t="s">
-        <v>343</v>
+        <v>455</v>
       </c>
       <c r="D224" s="29"/>
       <c r="E224" s="28"/>
@@ -8652,7 +8658,7 @@
         <v>1220101</v>
       </c>
       <c r="L224" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="225" spans="1:12" ht="18.75" customHeight="1">
@@ -8687,14 +8693,14 @@
         <v>2010101</v>
       </c>
       <c r="L225" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="226" spans="1:12" ht="18.75" customHeight="1">
       <c r="A226" s="33"/>
       <c r="B226" s="13"/>
       <c r="C226" s="13" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D226" s="29"/>
       <c r="E226" s="28"/>
@@ -8715,14 +8721,14 @@
         <v>2010102</v>
       </c>
       <c r="L226" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="227" spans="1:12" ht="18.75" customHeight="1">
       <c r="A227" s="23"/>
       <c r="B227" s="13"/>
       <c r="C227" s="13" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D227" s="29"/>
       <c r="E227" s="28"/>
@@ -8743,14 +8749,14 @@
         <v>2010103</v>
       </c>
       <c r="L227" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="228" spans="1:12" ht="18.75" customHeight="1">
       <c r="A228" s="23"/>
       <c r="B228" s="13"/>
       <c r="C228" s="13" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D228" s="29"/>
       <c r="E228" s="28"/>
@@ -8771,7 +8777,7 @@
         <v>2010104</v>
       </c>
       <c r="L228" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="229" spans="1:12" ht="18.75" customHeight="1">
@@ -8799,14 +8805,14 @@
         <v>2010105</v>
       </c>
       <c r="L229" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="230" spans="1:12" ht="18.75" customHeight="1">
       <c r="A230" s="23"/>
       <c r="B230" s="13"/>
       <c r="C230" s="13" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D230" s="29"/>
       <c r="E230" s="28"/>
@@ -8827,14 +8833,14 @@
         <v>2010106</v>
       </c>
       <c r="L230" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="231" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
       <c r="A231" s="23"/>
       <c r="B231" s="13"/>
       <c r="C231" s="14" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D231" s="29"/>
       <c r="E231" s="28"/>
@@ -8855,7 +8861,7 @@
         <v>2010107</v>
       </c>
       <c r="L231" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="232" spans="1:12" ht="18.75" customHeight="1">
@@ -8886,7 +8892,7 @@
         <v>2010201</v>
       </c>
       <c r="L232" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="233" spans="1:12" ht="18.75" customHeight="1">
@@ -8914,14 +8920,14 @@
         <v>2010202</v>
       </c>
       <c r="L233" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="234" spans="1:12" ht="18.75" customHeight="1">
       <c r="A234" s="23"/>
       <c r="B234" s="13"/>
       <c r="C234" s="17" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D234" s="29"/>
       <c r="E234" s="28"/>
@@ -8942,14 +8948,14 @@
         <v>2010203</v>
       </c>
       <c r="L234" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="235" spans="1:12" ht="18.75" customHeight="1">
       <c r="A235" s="23"/>
       <c r="B235" s="13"/>
       <c r="C235" s="17" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D235" s="29"/>
       <c r="E235" s="28"/>
@@ -8970,7 +8976,7 @@
         <v>2010204</v>
       </c>
       <c r="L235" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="236" spans="1:12" ht="18.75" customHeight="1">
@@ -8998,7 +9004,7 @@
         <v>2010205</v>
       </c>
       <c r="L236" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="237" spans="1:12" ht="18.75" customHeight="1">
@@ -9026,7 +9032,7 @@
         <v>2010206</v>
       </c>
       <c r="L237" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="238" spans="1:12" ht="18.75" customHeight="1">
@@ -9054,7 +9060,7 @@
         <v>2010207</v>
       </c>
       <c r="L238" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="239" spans="1:12" ht="18.75" customHeight="1">
@@ -9082,14 +9088,14 @@
         <v>2010208</v>
       </c>
       <c r="L239" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="240" spans="1:12" ht="18.75" customHeight="1">
       <c r="A240" s="23"/>
       <c r="B240" s="13"/>
       <c r="C240" s="17" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D240" s="29"/>
       <c r="E240" s="28"/>
@@ -9110,7 +9116,7 @@
         <v>2010209</v>
       </c>
       <c r="L240" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="241" spans="1:12" ht="18.75" customHeight="1">
@@ -9138,7 +9144,7 @@
         <v>2010210</v>
       </c>
       <c r="L241" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="242" spans="1:12" ht="18.75" customHeight="1">
@@ -9166,14 +9172,14 @@
         <v>2010211</v>
       </c>
       <c r="L242" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="243" spans="1:12" ht="18.75" customHeight="1">
       <c r="A243" s="23"/>
       <c r="B243" s="13"/>
       <c r="C243" s="17" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="D243" s="29"/>
       <c r="E243" s="28"/>
@@ -9194,7 +9200,7 @@
         <v>2010212</v>
       </c>
       <c r="L243" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="244" spans="1:12" ht="18.75" customHeight="1">
@@ -9222,14 +9228,14 @@
         <v>2010213</v>
       </c>
       <c r="L244" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="245" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
       <c r="A245" s="23"/>
       <c r="B245" s="13"/>
       <c r="C245" s="18" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D245" s="29"/>
       <c r="E245" s="28"/>
@@ -9250,18 +9256,18 @@
         <v>2010214</v>
       </c>
       <c r="L245" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="246" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
       <c r="A246" s="23"/>
       <c r="B246" s="14"/>
       <c r="C246" s="15" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="D246" s="29"/>
       <c r="E246" s="29" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="G246" s="40">
         <f t="shared" si="12"/>
@@ -9283,7 +9289,7 @@
         <v>2010301</v>
       </c>
       <c r="L246" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="247" spans="1:12" ht="18.75" customHeight="1">
@@ -9296,7 +9302,7 @@
       </c>
       <c r="D247" s="29"/>
       <c r="E247" s="29" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="F247" s="29"/>
       <c r="G247" s="40">
@@ -9319,20 +9325,20 @@
         <v>2020101</v>
       </c>
       <c r="L247" s="42" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="248" spans="1:12" ht="18.75" customHeight="1">
       <c r="A248" s="23"/>
       <c r="B248" s="17"/>
       <c r="C248" s="17" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D248" s="29" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="E248" s="29" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="F248" s="29"/>
       <c r="G248" s="40">
@@ -9352,7 +9358,7 @@
         <v>2020102</v>
       </c>
       <c r="L248" s="42" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="249" spans="1:12" ht="18.75" customHeight="1">
@@ -9363,7 +9369,7 @@
       </c>
       <c r="D249" s="29"/>
       <c r="E249" s="29" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="F249" s="29"/>
       <c r="G249" s="40">
@@ -9383,7 +9389,7 @@
         <v>2020103</v>
       </c>
       <c r="L249" s="42" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="250" spans="1:12" ht="18.75" customHeight="1">
@@ -9394,7 +9400,7 @@
       </c>
       <c r="D250" s="29"/>
       <c r="E250" s="29" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="F250" s="29"/>
       <c r="G250" s="40">
@@ -9414,7 +9420,7 @@
         <v>2020104</v>
       </c>
       <c r="L250" s="42" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="251" spans="1:12" ht="18.75" customHeight="1">
@@ -9425,7 +9431,7 @@
       </c>
       <c r="D251" s="29"/>
       <c r="E251" s="29" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="F251" s="29"/>
       <c r="G251" s="40">
@@ -9445,18 +9451,18 @@
         <v>2020105</v>
       </c>
       <c r="L251" s="42" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="252" spans="1:12" ht="18.75" customHeight="1">
       <c r="A252" s="23"/>
       <c r="B252" s="17"/>
       <c r="C252" s="17" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="D252" s="29"/>
       <c r="E252" s="29" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="F252" s="29"/>
       <c r="G252" s="40">
@@ -9476,20 +9482,20 @@
         <v>2020106</v>
       </c>
       <c r="L252" s="42" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="253" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
       <c r="A253" s="23"/>
       <c r="B253" s="17"/>
       <c r="C253" s="18" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D253" s="29" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="E253" s="29" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="F253" s="29"/>
       <c r="G253" s="40">
@@ -9509,7 +9515,7 @@
         <v>2020107</v>
       </c>
       <c r="L253" s="42" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="254" spans="1:12" ht="18.75" customHeight="1">
@@ -9520,7 +9526,7 @@
       </c>
       <c r="D254" s="29"/>
       <c r="E254" s="29" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="F254" s="29"/>
       <c r="G254" s="40">
@@ -9543,7 +9549,7 @@
         <v>2020201</v>
       </c>
       <c r="L254" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="255" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
@@ -9554,7 +9560,7 @@
       </c>
       <c r="D255" s="29"/>
       <c r="E255" s="29" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="F255" s="29"/>
       <c r="G255" s="40">
@@ -9574,7 +9580,7 @@
         <v>2020202</v>
       </c>
       <c r="L255" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="256" spans="1:12" ht="18.75" customHeight="1">
@@ -9585,7 +9591,7 @@
       </c>
       <c r="D256" s="29"/>
       <c r="E256" s="29" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="F256" s="29"/>
       <c r="G256" s="40">
@@ -9608,7 +9614,7 @@
         <v>2020301</v>
       </c>
       <c r="L256" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="257" spans="1:12" ht="18.75" customHeight="1">
@@ -9619,7 +9625,7 @@
       </c>
       <c r="D257" s="29"/>
       <c r="E257" s="29" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="F257" s="29"/>
       <c r="G257" s="40">
@@ -9639,7 +9645,7 @@
         <v>2020302</v>
       </c>
       <c r="L257" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="258" spans="1:12" ht="18.75" customHeight="1">
@@ -9650,7 +9656,7 @@
       </c>
       <c r="D258" s="29"/>
       <c r="E258" s="29" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="F258" s="29"/>
       <c r="G258" s="40">
@@ -9670,7 +9676,7 @@
         <v>2020303</v>
       </c>
       <c r="L258" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="259" spans="1:12" ht="18.75" customHeight="1">
@@ -9681,7 +9687,7 @@
       </c>
       <c r="D259" s="29"/>
       <c r="E259" s="29" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="F259" s="29"/>
       <c r="G259" s="40">
@@ -9701,18 +9707,18 @@
         <v>2020304</v>
       </c>
       <c r="L259" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="260" spans="1:12" ht="18.75" customHeight="1">
       <c r="A260" s="23"/>
       <c r="B260" s="24"/>
       <c r="C260" s="13" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D260" s="29"/>
       <c r="E260" s="29" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="F260" s="29"/>
       <c r="G260" s="40">
@@ -9732,18 +9738,18 @@
         <v>2020305</v>
       </c>
       <c r="L260" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="261" spans="1:12" ht="18.75" customHeight="1">
       <c r="A261" s="23"/>
       <c r="B261" s="24"/>
       <c r="C261" s="13" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D261" s="29"/>
       <c r="E261" s="29" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="F261" s="29"/>
       <c r="G261" s="40">
@@ -9763,18 +9769,18 @@
         <v>2020306</v>
       </c>
       <c r="L261" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="262" spans="1:12" ht="18.75" customHeight="1">
       <c r="A262" s="23"/>
       <c r="B262" s="24"/>
       <c r="C262" s="13" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="D262" s="29"/>
       <c r="E262" s="29" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="F262" s="29"/>
       <c r="G262" s="40">
@@ -9794,20 +9800,20 @@
         <v>2020307</v>
       </c>
       <c r="L262" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="263" spans="1:12" ht="18.75" customHeight="1">
       <c r="A263" s="23"/>
       <c r="B263" s="24"/>
       <c r="C263" s="13" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="D263" s="29" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="E263" s="29" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="F263" s="29"/>
       <c r="G263" s="40">
@@ -9827,7 +9833,7 @@
         <v>2020308</v>
       </c>
       <c r="L263" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="264" spans="1:12" ht="18.75" customHeight="1">
@@ -9838,7 +9844,7 @@
       </c>
       <c r="D264" s="29"/>
       <c r="E264" s="29" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="F264" s="29"/>
       <c r="G264" s="40">
@@ -9858,7 +9864,7 @@
         <v>2020309</v>
       </c>
       <c r="L264" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="265" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
@@ -9869,7 +9875,7 @@
       </c>
       <c r="D265" s="29"/>
       <c r="E265" s="29" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="F265" s="29"/>
       <c r="G265" s="40">
@@ -9889,18 +9895,18 @@
         <v>2020310</v>
       </c>
       <c r="L265" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="266" spans="1:12" ht="18.75" customHeight="1">
       <c r="A266" s="23"/>
       <c r="B266" s="17"/>
       <c r="C266" s="12" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D266" s="29"/>
       <c r="E266" s="29" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="F266" s="29"/>
       <c r="G266" s="40">
@@ -9923,18 +9929,18 @@
         <v>2020401</v>
       </c>
       <c r="L266" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="267" spans="1:12" ht="18.75" customHeight="1">
       <c r="A267" s="23"/>
       <c r="B267" s="24"/>
       <c r="C267" s="13" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D267" s="29"/>
       <c r="E267" s="29" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="F267" s="29"/>
       <c r="G267" s="40">
@@ -9954,18 +9960,18 @@
         <v>2020402</v>
       </c>
       <c r="L267" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="268" spans="1:12" ht="18.75" customHeight="1">
       <c r="A268" s="23"/>
       <c r="B268" s="17"/>
       <c r="C268" s="13" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D268" s="29"/>
       <c r="E268" s="29" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="F268" s="29"/>
       <c r="G268" s="40">
@@ -9985,18 +9991,18 @@
         <v>2020403</v>
       </c>
       <c r="L268" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="269" spans="1:12" ht="18.75" customHeight="1">
       <c r="A269" s="23"/>
       <c r="B269" s="17"/>
       <c r="C269" s="13" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D269" s="29"/>
       <c r="E269" s="29" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="F269" s="29"/>
       <c r="G269" s="40">
@@ -10016,18 +10022,18 @@
         <v>2020404</v>
       </c>
       <c r="L269" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="270" spans="1:12" ht="18.75" customHeight="1">
       <c r="A270" s="23"/>
       <c r="B270" s="17"/>
       <c r="C270" s="13" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D270" s="29"/>
       <c r="E270" s="29" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="F270" s="29"/>
       <c r="G270" s="40">
@@ -10047,18 +10053,18 @@
         <v>2020405</v>
       </c>
       <c r="L270" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="271" spans="1:12" ht="18.75" customHeight="1">
       <c r="A271" s="23"/>
       <c r="B271" s="17"/>
       <c r="C271" s="13" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="D271" s="29"/>
       <c r="E271" s="29" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="F271" s="29"/>
       <c r="G271" s="40">
@@ -10078,18 +10084,18 @@
         <v>2020406</v>
       </c>
       <c r="L271" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="272" spans="1:12" ht="18.75" customHeight="1">
       <c r="A272" s="23"/>
       <c r="B272" s="17"/>
       <c r="C272" s="13" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D272" s="29"/>
       <c r="E272" s="29" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="F272" s="29"/>
       <c r="G272" s="40">
@@ -10109,18 +10115,18 @@
         <v>2020407</v>
       </c>
       <c r="L272" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="273" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
       <c r="A273" s="23"/>
       <c r="B273" s="18"/>
       <c r="C273" s="13" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="D273" s="29"/>
       <c r="E273" s="29" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="F273" s="29"/>
       <c r="G273" s="40">
@@ -10140,20 +10146,20 @@
         <v>2020408</v>
       </c>
       <c r="L273" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="274" spans="1:12" ht="18.75" customHeight="1">
       <c r="A274" s="23"/>
       <c r="B274" s="12" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C274" s="12" t="s">
         <v>54</v>
       </c>
       <c r="D274" s="29"/>
       <c r="E274" s="29" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="F274" s="29"/>
       <c r="G274" s="40">
@@ -10176,7 +10182,7 @@
         <v>2030101</v>
       </c>
       <c r="L274" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="275" spans="1:12" ht="18.75" customHeight="1">
@@ -10187,7 +10193,7 @@
       </c>
       <c r="D275" s="29"/>
       <c r="E275" s="29" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="F275" s="29"/>
       <c r="G275" s="40">
@@ -10207,7 +10213,7 @@
         <v>2030102</v>
       </c>
       <c r="L275" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="276" spans="1:12" ht="18.75" customHeight="1">
@@ -10218,7 +10224,7 @@
       </c>
       <c r="D276" s="29"/>
       <c r="E276" s="29" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="F276" s="29"/>
       <c r="G276" s="40">
@@ -10238,7 +10244,7 @@
         <v>2030103</v>
       </c>
       <c r="L276" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="277" spans="1:12" ht="18.75" customHeight="1">
@@ -10249,7 +10255,7 @@
       </c>
       <c r="D277" s="29"/>
       <c r="E277" s="29" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="F277" s="29"/>
       <c r="G277" s="40">
@@ -10269,7 +10275,7 @@
         <v>2030104</v>
       </c>
       <c r="L277" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="278" spans="1:12" ht="18.75" customHeight="1">
@@ -10280,7 +10286,7 @@
       </c>
       <c r="D278" s="29"/>
       <c r="E278" s="29" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="F278" s="29"/>
       <c r="G278" s="40">
@@ -10300,18 +10306,18 @@
         <v>2030105</v>
       </c>
       <c r="L278" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="279" spans="1:12" ht="18.75" customHeight="1">
       <c r="A279" s="23"/>
       <c r="B279" s="13"/>
       <c r="C279" s="13" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D279" s="29"/>
       <c r="E279" s="29" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="F279" s="29"/>
       <c r="G279" s="40">
@@ -10331,7 +10337,7 @@
         <v>2030106</v>
       </c>
       <c r="L279" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="280" spans="1:12" ht="18.75" customHeight="1">
@@ -10342,7 +10348,7 @@
       </c>
       <c r="D280" s="29"/>
       <c r="E280" s="29" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="F280" s="29"/>
       <c r="G280" s="40">
@@ -10362,7 +10368,7 @@
         <v>2030107</v>
       </c>
       <c r="L280" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="281" spans="1:12" ht="18.75" customHeight="1">
@@ -10373,7 +10379,7 @@
       </c>
       <c r="D281" s="29"/>
       <c r="E281" s="29" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="F281" s="29"/>
       <c r="G281" s="40">
@@ -10393,7 +10399,7 @@
         <v>2030108</v>
       </c>
       <c r="L281" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="282" spans="1:12" ht="18.75" customHeight="1">
@@ -10404,7 +10410,7 @@
       </c>
       <c r="D282" s="29"/>
       <c r="E282" s="29" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="F282" s="29"/>
       <c r="G282" s="40">
@@ -10424,20 +10430,20 @@
         <v>2030109</v>
       </c>
       <c r="L282" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="283" spans="1:12" ht="18.75" customHeight="1">
       <c r="A283" s="23"/>
       <c r="B283" s="13"/>
       <c r="C283" s="13" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="D283" s="29" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="E283" s="29" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="F283" s="29"/>
       <c r="G283" s="40">
@@ -10457,18 +10463,18 @@
         <v>2030110</v>
       </c>
       <c r="L283" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="284" spans="1:12" ht="18.75" customHeight="1">
       <c r="A284" s="23"/>
       <c r="B284" s="13"/>
       <c r="C284" s="13" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D284" s="29"/>
       <c r="E284" s="29" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="F284" s="29"/>
       <c r="G284" s="40">
@@ -10488,18 +10494,18 @@
         <v>2030111</v>
       </c>
       <c r="L284" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="285" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
       <c r="A285" s="23"/>
       <c r="B285" s="13"/>
       <c r="C285" s="14" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D285" s="29"/>
       <c r="E285" s="29" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="F285" s="29"/>
       <c r="G285" s="40">
@@ -10519,7 +10525,7 @@
         <v>2030112</v>
       </c>
       <c r="L285" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="286" spans="1:12" ht="18.75" customHeight="1">
@@ -10550,17 +10556,17 @@
         <v>2030201</v>
       </c>
       <c r="L286" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="287" spans="1:12" ht="18.75" customHeight="1">
       <c r="A287" s="23"/>
       <c r="B287" s="13"/>
       <c r="C287" s="13" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D287" s="29" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="E287" s="28"/>
       <c r="G287" s="40">
@@ -10580,14 +10586,14 @@
         <v>2030202</v>
       </c>
       <c r="L287" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="288" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
       <c r="A288" s="23"/>
       <c r="B288" s="14"/>
       <c r="C288" s="14" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D288" s="29"/>
       <c r="E288" s="28"/>
@@ -10608,13 +10614,13 @@
         <v>2030203</v>
       </c>
       <c r="L288" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="289" spans="1:12" ht="18.75" customHeight="1">
       <c r="A289" s="23"/>
       <c r="B289" s="17" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C289" s="17" t="s">
         <v>22</v>
@@ -10641,14 +10647,14 @@
         <v>2050101</v>
       </c>
       <c r="L289" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="290" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
       <c r="A290" s="23"/>
       <c r="B290" s="18"/>
       <c r="C290" s="18" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="D290" s="29"/>
       <c r="E290" s="28"/>
@@ -10669,16 +10675,16 @@
         <v>2050102</v>
       </c>
       <c r="L290" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="291" spans="1:12" ht="18.75" customHeight="1">
       <c r="A291" s="23"/>
       <c r="B291" s="17" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C291" s="17" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D291" s="29"/>
       <c r="E291" s="28"/>
@@ -10702,14 +10708,14 @@
         <v>2040101</v>
       </c>
       <c r="L291" s="42" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="292" spans="1:12" ht="18.75" customHeight="1">
       <c r="A292" s="23"/>
       <c r="B292" s="17"/>
       <c r="C292" s="17" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="D292" s="29"/>
       <c r="E292" s="28"/>
@@ -10730,7 +10736,7 @@
         <v>2040102</v>
       </c>
       <c r="L292" s="42" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="293" spans="1:12" ht="18.75" customHeight="1">
@@ -10758,7 +10764,7 @@
         <v>2040103</v>
       </c>
       <c r="L293" s="42" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="294" spans="1:12" ht="18.75" customHeight="1">
@@ -10786,7 +10792,7 @@
         <v>2040104</v>
       </c>
       <c r="L294" s="42" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="295" spans="1:12" ht="18.75" customHeight="1">
@@ -10814,7 +10820,7 @@
         <v>2040105</v>
       </c>
       <c r="L295" s="42" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="296" spans="1:12" ht="18.75" customHeight="1">
@@ -10842,7 +10848,7 @@
         <v>2040106</v>
       </c>
       <c r="L296" s="42" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="297" spans="1:12" ht="18.75" customHeight="1">
@@ -10870,7 +10876,7 @@
         <v>2040107</v>
       </c>
       <c r="L297" s="42" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="298" spans="1:12" ht="18.75" customHeight="1">
@@ -10898,7 +10904,7 @@
         <v>2040108</v>
       </c>
       <c r="L298" s="42" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="299" spans="1:12" ht="18.75" customHeight="1">
@@ -10926,7 +10932,7 @@
         <v>2040109</v>
       </c>
       <c r="L299" s="42" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="300" spans="1:12" ht="18.75" customHeight="1">
@@ -10954,7 +10960,7 @@
         <v>2040110</v>
       </c>
       <c r="L300" s="42" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="301" spans="1:12" ht="18.75" customHeight="1">
@@ -10982,14 +10988,14 @@
         <v>2040111</v>
       </c>
       <c r="L301" s="42" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="302" spans="1:12" ht="18.75" customHeight="1">
       <c r="A302" s="23"/>
       <c r="B302" s="17"/>
       <c r="C302" s="17" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D302" s="29"/>
       <c r="E302" s="28"/>
@@ -11010,14 +11016,14 @@
         <v>2040112</v>
       </c>
       <c r="L302" s="42" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="303" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
       <c r="A303" s="23"/>
       <c r="B303" s="18"/>
       <c r="C303" s="18" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="D303" s="29"/>
       <c r="E303" s="28"/>
@@ -11038,7 +11044,7 @@
         <v>2040113</v>
       </c>
       <c r="L303" s="42" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="304" spans="1:12" ht="18.75" customHeight="1">
@@ -11071,14 +11077,14 @@
         <v>2060101</v>
       </c>
       <c r="L304" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="305" spans="1:12" ht="18.75" customHeight="1">
       <c r="A305" s="23"/>
       <c r="B305" s="17"/>
       <c r="C305" s="17" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="D305" s="29"/>
       <c r="E305" s="28"/>
@@ -11099,7 +11105,7 @@
         <v>2060102</v>
       </c>
       <c r="L305" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="306" spans="1:12" ht="18.75" customHeight="1">
@@ -11127,14 +11133,14 @@
         <v>2060103</v>
       </c>
       <c r="L306" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="307" spans="1:12" ht="18.75" customHeight="1">
       <c r="A307" s="23"/>
       <c r="B307" s="17"/>
       <c r="C307" s="17" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D307" s="29"/>
       <c r="E307" s="28"/>
@@ -11155,14 +11161,14 @@
         <v>2060104</v>
       </c>
       <c r="L307" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="308" spans="1:12" ht="18.75" customHeight="1">
       <c r="A308" s="23"/>
       <c r="B308" s="17"/>
       <c r="C308" s="17" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D308" s="29"/>
       <c r="E308" s="28"/>
@@ -11183,14 +11189,14 @@
         <v>2060105</v>
       </c>
       <c r="L308" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="309" spans="1:12" ht="18.75" customHeight="1">
       <c r="A309" s="23"/>
       <c r="B309" s="17"/>
       <c r="C309" s="17" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D309" s="29"/>
       <c r="E309" s="28"/>
@@ -11211,17 +11217,17 @@
         <v>2060106</v>
       </c>
       <c r="L309" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="310" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
       <c r="A310" s="23"/>
       <c r="B310" s="17"/>
       <c r="C310" s="18" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D310" s="29" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="E310" s="28"/>
       <c r="G310" s="40">
@@ -11241,7 +11247,7 @@
         <v>2060107</v>
       </c>
       <c r="L310" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="311" spans="1:12" ht="18.75" customHeight="1">
@@ -11272,7 +11278,7 @@
         <v>2060201</v>
       </c>
       <c r="L311" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="312" spans="1:12" ht="18.75" customHeight="1">
@@ -11300,14 +11306,14 @@
         <v>2060202</v>
       </c>
       <c r="L312" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="313" spans="1:12" ht="18.75" customHeight="1">
       <c r="A313" s="23"/>
       <c r="B313" s="17"/>
       <c r="C313" s="17" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="D313" s="29"/>
       <c r="E313" s="28"/>
@@ -11328,14 +11334,14 @@
         <v>2060203</v>
       </c>
       <c r="L313" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="314" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
       <c r="A314" s="23"/>
       <c r="B314" s="17"/>
       <c r="C314" s="17" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="D314" s="29"/>
       <c r="E314" s="28"/>
@@ -11356,7 +11362,7 @@
         <v>2060204</v>
       </c>
       <c r="L314" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="315" spans="1:12" ht="18.75" customHeight="1">
@@ -11389,17 +11395,17 @@
         <v>2070101</v>
       </c>
       <c r="L315" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="316" spans="1:12" ht="18.75" customHeight="1">
       <c r="A316" s="23"/>
       <c r="B316" s="13"/>
       <c r="C316" s="13" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D316" s="29" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="E316" s="28"/>
       <c r="G316" s="40">
@@ -11419,7 +11425,7 @@
         <v>2070102</v>
       </c>
       <c r="L316" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="317" spans="1:12" ht="18.75" customHeight="1">
@@ -11447,7 +11453,7 @@
         <v>2070103</v>
       </c>
       <c r="L317" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="318" spans="1:12" ht="18.75" customHeight="1">
@@ -11475,7 +11481,7 @@
         <v>2070104</v>
       </c>
       <c r="L318" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="319" spans="1:12" ht="18.75" customHeight="1">
@@ -11503,14 +11509,14 @@
         <v>2070105</v>
       </c>
       <c r="L319" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="320" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
       <c r="A320" s="23"/>
       <c r="B320" s="14"/>
       <c r="C320" s="14" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="D320" s="29"/>
       <c r="E320" s="28"/>
@@ -11531,16 +11537,16 @@
         <v>2070106</v>
       </c>
       <c r="L320" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="321" spans="1:12" ht="18.75" customHeight="1">
       <c r="A321" s="23"/>
       <c r="B321" s="17" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="C321" s="17" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="D321" s="29"/>
       <c r="E321" s="28"/>
@@ -11564,14 +11570,14 @@
         <v>2080101</v>
       </c>
       <c r="L321" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="322" spans="1:12" ht="18.75" customHeight="1">
       <c r="A322" s="23"/>
       <c r="B322" s="17"/>
       <c r="C322" s="17" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="D322" s="29"/>
       <c r="E322" s="28"/>
@@ -11592,14 +11598,14 @@
         <v>2080102</v>
       </c>
       <c r="L322" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="323" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
       <c r="A323" s="23"/>
       <c r="B323" s="18"/>
       <c r="C323" s="18" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="D323" s="29"/>
       <c r="E323" s="28"/>
@@ -11620,7 +11626,7 @@
         <v>2080103</v>
       </c>
       <c r="L323" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="324" spans="1:12" ht="18.75" customHeight="1">
@@ -11629,7 +11635,7 @@
         <v>144</v>
       </c>
       <c r="C324" s="17" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D324" s="29"/>
       <c r="E324" s="28"/>
@@ -11653,17 +11659,17 @@
         <v>2100101</v>
       </c>
       <c r="L324" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="325" spans="1:12" ht="18.75" customHeight="1">
       <c r="A325" s="23"/>
       <c r="B325" s="17"/>
       <c r="C325" s="17" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="D325" s="29" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="E325" s="28"/>
       <c r="G325" s="40">
@@ -11683,14 +11689,14 @@
         <v>2100102</v>
       </c>
       <c r="L325" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="326" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
       <c r="A326" s="23"/>
       <c r="B326" s="18"/>
       <c r="C326" s="18" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="D326" s="29"/>
       <c r="E326" s="28"/>
@@ -11711,7 +11717,7 @@
         <v>2100103</v>
       </c>
       <c r="L326" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="327" spans="1:12" ht="18.75" customHeight="1">
@@ -11720,10 +11726,10 @@
         <v>142</v>
       </c>
       <c r="C327" s="12" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="D327" s="29" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="E327" s="28"/>
       <c r="G327" s="40">
@@ -11746,17 +11752,17 @@
         <v>2090101</v>
       </c>
       <c r="L327" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="328" spans="1:12" ht="18.75" customHeight="1">
       <c r="A328" s="23"/>
       <c r="B328" s="13"/>
       <c r="C328" s="13" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="D328" s="29" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="E328" s="28"/>
       <c r="G328" s="40">
@@ -11776,14 +11782,14 @@
         <v>2090102</v>
       </c>
       <c r="L328" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="329" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
       <c r="A329" s="23"/>
       <c r="B329" s="14"/>
       <c r="C329" s="14" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D329" s="29"/>
       <c r="E329" s="28"/>
@@ -11804,7 +11810,7 @@
         <v>2090103</v>
       </c>
       <c r="L329" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="330" spans="1:12" ht="18.75" customHeight="1">
@@ -11837,14 +11843,14 @@
         <v>2110101</v>
       </c>
       <c r="L330" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="331" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
       <c r="A331" s="23"/>
       <c r="B331" s="14"/>
       <c r="C331" s="14" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D331" s="29"/>
       <c r="E331" s="28"/>
@@ -11865,7 +11871,7 @@
         <v>2110102</v>
       </c>
       <c r="L331" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="332" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
@@ -11874,7 +11880,7 @@
         <v>153</v>
       </c>
       <c r="C332" s="18" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="D332" s="29"/>
       <c r="E332" s="28"/>
@@ -11898,16 +11904,16 @@
         <v>2120101</v>
       </c>
       <c r="L332" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="333" spans="1:12" ht="18.75" customHeight="1">
       <c r="A333" s="23"/>
       <c r="B333" s="17" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C333" s="17" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="D333" s="29"/>
       <c r="E333" s="28"/>
@@ -11931,14 +11937,14 @@
         <v>2130101</v>
       </c>
       <c r="L333" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="334" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
       <c r="A334" s="23"/>
       <c r="B334" s="17"/>
       <c r="C334" s="17" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="D334" s="29"/>
       <c r="E334" s="28"/>
@@ -11959,7 +11965,7 @@
         <v>2130102</v>
       </c>
       <c r="L334" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="335" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
@@ -11992,13 +11998,13 @@
         <v>2140101</v>
       </c>
       <c r="L335" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="336" spans="1:12" ht="18.75" customHeight="1">
       <c r="A336" s="23"/>
       <c r="B336" s="12" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C336" s="12" t="s">
         <v>190</v>
@@ -12025,7 +12031,7 @@
         <v>2150101</v>
       </c>
       <c r="L336" s="42" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="337" spans="1:12" ht="18.75" customHeight="1">
@@ -12053,7 +12059,7 @@
         <v>2150102</v>
       </c>
       <c r="L337" s="42" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="338" spans="1:12" ht="18.75" customHeight="1">
@@ -12081,7 +12087,7 @@
         <v>2150103</v>
       </c>
       <c r="L338" s="42" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="339" spans="1:12" ht="18.75" customHeight="1">
@@ -12109,14 +12115,14 @@
         <v>2150104</v>
       </c>
       <c r="L339" s="42" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="340" spans="1:12" ht="18.75" customHeight="1">
       <c r="A340" s="23"/>
       <c r="B340" s="13"/>
       <c r="C340" s="13" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="D340" s="29"/>
       <c r="E340" s="28"/>
@@ -12137,7 +12143,7 @@
         <v>2150105</v>
       </c>
       <c r="L340" s="42" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="341" spans="1:12" ht="18.75" customHeight="1">
@@ -12165,14 +12171,14 @@
         <v>2150106</v>
       </c>
       <c r="L341" s="42" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="342" spans="1:12" ht="18.75" customHeight="1">
       <c r="A342" s="23"/>
       <c r="B342" s="13"/>
       <c r="C342" s="13" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D342" s="29"/>
       <c r="E342" s="28"/>
@@ -12193,7 +12199,7 @@
         <v>2150107</v>
       </c>
       <c r="L342" s="42" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="343" spans="1:12" ht="18.75" customHeight="1">
@@ -12221,14 +12227,14 @@
         <v>2150108</v>
       </c>
       <c r="L343" s="42" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="344" spans="1:12" ht="18.75" customHeight="1">
       <c r="A344" s="23"/>
       <c r="B344" s="13"/>
       <c r="C344" s="13" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="D344" s="29"/>
       <c r="E344" s="28"/>
@@ -12249,14 +12255,14 @@
         <v>2150109</v>
       </c>
       <c r="L344" s="42" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="345" spans="1:12" ht="18.75" customHeight="1">
       <c r="A345" s="23"/>
       <c r="B345" s="13"/>
       <c r="C345" s="13" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="D345" s="29"/>
       <c r="E345" s="28"/>
@@ -12277,7 +12283,7 @@
         <v>2150110</v>
       </c>
       <c r="L345" s="42" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="346" spans="1:12" ht="18.75" customHeight="1">
@@ -12305,14 +12311,14 @@
         <v>2150111</v>
       </c>
       <c r="L346" s="42" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="347" spans="1:12" ht="18.75" customHeight="1">
       <c r="A347" s="23"/>
       <c r="B347" s="13"/>
       <c r="C347" s="13" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="D347" s="29"/>
       <c r="E347" s="28"/>
@@ -12333,7 +12339,7 @@
         <v>2150112</v>
       </c>
       <c r="L347" s="42" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="348" spans="1:12" ht="18.75" customHeight="1">
@@ -12361,14 +12367,14 @@
         <v>2150113</v>
       </c>
       <c r="L348" s="42" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="349" spans="1:12" ht="18.75" customHeight="1">
       <c r="A349" s="23"/>
       <c r="B349" s="13"/>
       <c r="C349" s="13" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="D349" s="29"/>
       <c r="E349" s="28"/>
@@ -12389,14 +12395,14 @@
         <v>2150114</v>
       </c>
       <c r="L349" s="42" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="350" spans="1:12" ht="18.75" customHeight="1">
       <c r="A350" s="23"/>
       <c r="B350" s="13"/>
       <c r="C350" s="13" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="D350" s="29"/>
       <c r="E350" s="28"/>
@@ -12417,7 +12423,7 @@
         <v>2150115</v>
       </c>
       <c r="L350" s="42" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="351" spans="1:12" ht="18.75" customHeight="1">
@@ -12445,14 +12451,14 @@
         <v>2150116</v>
       </c>
       <c r="L351" s="42" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="352" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
       <c r="A352" s="23"/>
       <c r="B352" s="13"/>
       <c r="C352" s="13" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="D352" s="29"/>
       <c r="E352" s="28"/>
@@ -12473,16 +12479,16 @@
         <v>2150117</v>
       </c>
       <c r="L352" s="42" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="353" spans="1:12" ht="18.75" customHeight="1">
       <c r="A353" s="23"/>
       <c r="B353" s="26" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C353" s="12" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="D353" s="29"/>
       <c r="E353" s="28"/>
@@ -12506,14 +12512,14 @@
         <v>2160101</v>
       </c>
       <c r="L353" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="354" spans="1:12" ht="18.75" customHeight="1">
       <c r="A354" s="23"/>
       <c r="B354" s="13"/>
       <c r="C354" s="39" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="D354" s="29"/>
       <c r="E354" s="28"/>
@@ -12534,14 +12540,14 @@
         <v>2160102</v>
       </c>
       <c r="L354" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="355" spans="1:12" ht="18.75" customHeight="1">
       <c r="A355" s="23"/>
       <c r="B355" s="13"/>
       <c r="C355" s="39" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="D355" s="29"/>
       <c r="E355" s="28"/>
@@ -12562,7 +12568,7 @@
         <v>2160103</v>
       </c>
       <c r="L355" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="356" spans="1:12" ht="18.75" customHeight="1">
@@ -12590,7 +12596,7 @@
         <v>2160104</v>
       </c>
       <c r="L356" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="357" spans="1:12" ht="18.75" customHeight="1">
@@ -12618,14 +12624,14 @@
         <v>2160105</v>
       </c>
       <c r="L357" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="358" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
       <c r="A358" s="23"/>
       <c r="B358" s="13"/>
       <c r="C358" s="14" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="D358" s="29"/>
       <c r="E358" s="28"/>
@@ -12646,16 +12652,16 @@
         <v>2160106</v>
       </c>
       <c r="L358" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="359" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
       <c r="A359" s="23"/>
       <c r="B359" s="19" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C359" s="19" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="D359" s="29"/>
       <c r="E359" s="28"/>
@@ -12679,16 +12685,16 @@
         <v>2170101</v>
       </c>
       <c r="L359" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="360" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
       <c r="A360" s="23"/>
       <c r="B360" s="15" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="C360" s="15" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="D360" s="29"/>
       <c r="E360" s="28"/>
@@ -12712,16 +12718,16 @@
         <v>2180101</v>
       </c>
       <c r="L360" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="361" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
       <c r="A361" s="18"/>
       <c r="B361" s="19" t="s">
-        <v>447</v>
+        <v>453</v>
       </c>
       <c r="C361" s="19" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="D361" s="29"/>
       <c r="E361" s="28"/>
@@ -12745,7 +12751,7 @@
         <v>2190101</v>
       </c>
       <c r="L361" s="42" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
   </sheetData>

</xml_diff>